<commit_message>
start of switching DE source
</commit_message>
<xml_diff>
--- a/data/cases-de.xlsx
+++ b/data/cases-de.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/torben/Hacken/GitHub/COVID-19-Coronavirus-German-Regions/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A9C38B9-B26F-944A-97A5-459F166F87FF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49665D7F-AC9C-4A49-99CE-ACA9B0829AED}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="80" yWindow="460" windowWidth="25440" windowHeight="14300" xr2:uid="{309167EE-B9E7-9F44-B3F3-07C1908B9528}"/>
+    <workbookView xWindow="80" yWindow="460" windowWidth="25440" windowHeight="14300" activeTab="6" xr2:uid="{309167EE-B9E7-9F44-B3F3-07C1908B9528}"/>
   </bookViews>
   <sheets>
     <sheet name="Links" sheetId="10" r:id="rId1"/>
@@ -127,7 +127,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="365" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="367" uniqueCount="104">
   <si>
     <t>Baden-Württemberg</t>
   </si>
@@ -432,6 +432,21 @@
     <t>Model: Verdopplung
 alle 3 Tage</t>
   </si>
+  <si>
+    <t>Baden-Württem­berg</t>
+  </si>
+  <si>
+    <t>Mecklenburg-Vor­pommern</t>
+  </si>
+  <si>
+    <t>Nordrhein-West­falen</t>
+  </si>
+  <si>
+    <t>Rhein­land-Pfalz</t>
+  </si>
+  <si>
+    <t>Schles­wig-Holstein</t>
+  </si>
 </sst>
 </file>
 
@@ -656,7 +671,7 @@
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="114">
+  <cellXfs count="116">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -850,9 +865,6 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -891,6 +903,9 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="90"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
@@ -2503,10 +2518,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Cases!$B$2:$B$23</c:f>
+              <c:f>Cases!$B$2:$B$24</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy\ h:mm</c:formatCode>
-                <c:ptCount val="22"/>
+                <c:ptCount val="23"/>
                 <c:pt idx="0">
                   <c:v>43889.416666666664</c:v>
                 </c:pt>
@@ -2572,16 +2587,19 @@
                 </c:pt>
                 <c:pt idx="21">
                   <c:v>43910</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>43911</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Cases!$T$2:$T$23</c:f>
+              <c:f>Cases!$T$2:$T$24</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="22"/>
+                <c:ptCount val="23"/>
                 <c:pt idx="0">
                   <c:v>53</c:v>
                 </c:pt>
@@ -2647,6 +2665,9 @@
                 </c:pt>
                 <c:pt idx="21">
                   <c:v>13957</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>16662</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2691,10 +2712,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Cases!$B$2:$B$23</c:f>
+              <c:f>Cases!$B$2:$B$24</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy\ h:mm</c:formatCode>
-                <c:ptCount val="22"/>
+                <c:ptCount val="23"/>
                 <c:pt idx="0">
                   <c:v>43889.416666666664</c:v>
                 </c:pt>
@@ -2760,78 +2781,87 @@
                 </c:pt>
                 <c:pt idx="21">
                   <c:v>43910</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>43911</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Cases!$W$2:$W$23</c:f>
+              <c:f>Cases!$W$2:$W$24</c:f>
               <c:numCache>
                 <c:formatCode>0</c:formatCode>
-                <c:ptCount val="22"/>
+                <c:ptCount val="23"/>
+                <c:pt idx="0">
+                  <c:v>56.879209835213864</c:v>
+                </c:pt>
                 <c:pt idx="1">
-                  <c:v>75.631927159515868</c:v>
+                  <c:v>71.663313772773421</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>99.989261179746862</c:v>
+                  <c:v>94.742552080142715</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>125.97857492379933</c:v>
+                  <c:v>119.36813568653308</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>158.72305838225327</c:v>
+                  <c:v>150.3944268381704</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>199.97852235949375</c:v>
+                  <c:v>189.48510416028546</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>251.95714984759874</c:v>
+                  <c:v>238.73627137306619</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>317.44611676450643</c:v>
+                  <c:v>300.78885367634092</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>399.9570447189875</c:v>
+                  <c:v>378.97020832057075</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>503.91429969519737</c:v>
+                  <c:v>477.47254274613243</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>634.89223352901297</c:v>
+                  <c:v>601.57770735268173</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>799.91408943797478</c:v>
+                  <c:v>757.94041664114161</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>1007.8285993903947</c:v>
+                  <c:v>954.94508549226452</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>1269.7844670580257</c:v>
+                  <c:v>1203.1554147053635</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>1599.8281788759496</c:v>
+                  <c:v>1515.880833282283</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>2015.6571987807893</c:v>
+                  <c:v>1909.890170984529</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>2539.5689341160519</c:v>
+                  <c:v>2406.3108294107265</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>3199.6563577518991</c:v>
+                  <c:v>3031.7616665645664</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>4031.314397561579</c:v>
+                  <c:v>3819.7803419690581</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>4396.179523345686</c:v>
+                  <c:v>4165.5</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>5538.8391205800408</c:v>
+                  <c:v>5248.2011333370947</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>6978.5</c:v>
+                  <c:v>6612.3190819735355</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>8331</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2884,10 +2914,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Cases!$B$2:$B$23</c:f>
+              <c:f>Cases!$B$2:$B$24</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy\ h:mm</c:formatCode>
-                <c:ptCount val="22"/>
+                <c:ptCount val="23"/>
                 <c:pt idx="0">
                   <c:v>43889.416666666664</c:v>
                 </c:pt>
@@ -2953,16 +2983,19 @@
                 </c:pt>
                 <c:pt idx="21">
                   <c:v>43910</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>43911</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Cases!$M$2:$M$23</c:f>
+              <c:f>Cases!$M$2:$M$24</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="22"/>
+                <c:ptCount val="23"/>
                 <c:pt idx="0">
                   <c:v>25</c:v>
                 </c:pt>
@@ -3028,6 +3061,9 @@
                 </c:pt>
                 <c:pt idx="21">
                   <c:v>3497</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>3542</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3079,10 +3115,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Cases!$B$2:$B$23</c:f>
+              <c:f>Cases!$B$2:$B$24</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy\ h:mm</c:formatCode>
-                <c:ptCount val="22"/>
+                <c:ptCount val="23"/>
                 <c:pt idx="0">
                   <c:v>43889.416666666664</c:v>
                 </c:pt>
@@ -3148,16 +3184,19 @@
                 </c:pt>
                 <c:pt idx="21">
                   <c:v>43910</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>43911</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Cases!$E$2:$E$23</c:f>
+              <c:f>Cases!$E$2:$E$24</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="22"/>
+                <c:ptCount val="23"/>
                 <c:pt idx="0">
                   <c:v>15</c:v>
                 </c:pt>
@@ -3223,6 +3262,9 @@
                 </c:pt>
                 <c:pt idx="21">
                   <c:v>2401</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>2960</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3275,10 +3317,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Cases!$B$2:$B$23</c:f>
+              <c:f>Cases!$B$2:$B$24</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy\ h:mm</c:formatCode>
-                <c:ptCount val="22"/>
+                <c:ptCount val="23"/>
                 <c:pt idx="0">
                   <c:v>43889.416666666664</c:v>
                 </c:pt>
@@ -3344,16 +3386,19 @@
                 </c:pt>
                 <c:pt idx="21">
                   <c:v>43910</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>43911</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Cases!$D$2:$D$23</c:f>
+              <c:f>Cases!$D$2:$D$24</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="22"/>
+                <c:ptCount val="23"/>
                 <c:pt idx="0">
                   <c:v>10</c:v>
                 </c:pt>
@@ -3419,6 +3464,9 @@
                 </c:pt>
                 <c:pt idx="21">
                   <c:v>2746</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>3668</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3470,10 +3518,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Cases!$B$2:$B$23</c:f>
+              <c:f>Cases!$B$2:$B$24</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy\ h:mm</c:formatCode>
-                <c:ptCount val="22"/>
+                <c:ptCount val="23"/>
                 <c:pt idx="0">
                   <c:v>43889.416666666664</c:v>
                 </c:pt>
@@ -3539,16 +3587,19 @@
                 </c:pt>
                 <c:pt idx="21">
                   <c:v>43910</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>43911</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Cases!$L$2:$L$23</c:f>
+              <c:f>Cases!$L$2:$L$24</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="22"/>
+                <c:ptCount val="23"/>
                 <c:pt idx="2">
                   <c:v>1</c:v>
                 </c:pt>
@@ -3608,6 +3659,9 @@
                 </c:pt>
                 <c:pt idx="21">
                   <c:v>803</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>1023</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3665,10 +3719,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Cases!$B$2:$B$23</c:f>
+              <c:f>Cases!$B$2:$B$24</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy\ h:mm</c:formatCode>
-                <c:ptCount val="22"/>
+                <c:ptCount val="23"/>
                 <c:pt idx="0">
                   <c:v>43889.416666666664</c:v>
                 </c:pt>
@@ -3734,16 +3788,19 @@
                 </c:pt>
                 <c:pt idx="21">
                   <c:v>43910</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>43911</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Cases!$F$2:$F$23</c:f>
+              <c:f>Cases!$F$2:$F$24</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="22"/>
+                <c:ptCount val="23"/>
                 <c:pt idx="3">
                   <c:v>1</c:v>
                 </c:pt>
@@ -3800,6 +3857,9 @@
                 </c:pt>
                 <c:pt idx="21">
                   <c:v>731</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>866</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3857,10 +3917,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Cases!$B$2:$B$23</c:f>
+              <c:f>Cases!$B$2:$B$24</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy\ h:mm</c:formatCode>
-                <c:ptCount val="22"/>
+                <c:ptCount val="23"/>
                 <c:pt idx="0">
                   <c:v>43889.416666666664</c:v>
                 </c:pt>
@@ -3926,16 +3986,19 @@
                 </c:pt>
                 <c:pt idx="21">
                   <c:v>43910</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>43911</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Cases!$J$2:$J$23</c:f>
+              <c:f>Cases!$J$2:$J$24</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="22"/>
+                <c:ptCount val="23"/>
                 <c:pt idx="1">
                   <c:v>3</c:v>
                 </c:pt>
@@ -3998,6 +4061,9 @@
                 </c:pt>
                 <c:pt idx="21">
                   <c:v>813</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>1080</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4055,10 +4121,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Cases!$B$2:$B$23</c:f>
+              <c:f>Cases!$B$2:$B$24</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy\ h:mm</c:formatCode>
-                <c:ptCount val="22"/>
+                <c:ptCount val="23"/>
                 <c:pt idx="0">
                   <c:v>43889.416666666664</c:v>
                 </c:pt>
@@ -4124,16 +4190,19 @@
                 </c:pt>
                 <c:pt idx="21">
                   <c:v>43910</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>43911</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Cases!$I$2:$I$23</c:f>
+              <c:f>Cases!$I$2:$I$24</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="22"/>
+                <c:ptCount val="23"/>
                 <c:pt idx="2">
                   <c:v>1</c:v>
                 </c:pt>
@@ -4193,6 +4262,9 @@
                 </c:pt>
                 <c:pt idx="21">
                   <c:v>586</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>587</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4254,10 +4326,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Cases!$B$2:$B$23</c:f>
+              <c:f>Cases!$B$2:$B$24</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy\ h:mm</c:formatCode>
-                <c:ptCount val="22"/>
+                <c:ptCount val="23"/>
                 <c:pt idx="0">
                   <c:v>43889.416666666664</c:v>
                 </c:pt>
@@ -4323,16 +4395,19 @@
                 </c:pt>
                 <c:pt idx="21">
                   <c:v>43910</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>43911</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Cases!$N$2:$N$23</c:f>
+              <c:f>Cases!$N$2:$N$24</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="22"/>
+                <c:ptCount val="23"/>
                 <c:pt idx="0">
                   <c:v>2</c:v>
                 </c:pt>
@@ -4398,6 +4473,9 @@
                 </c:pt>
                 <c:pt idx="21">
                   <c:v>801</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>938</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4449,10 +4527,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Cases!$B$2:$B$23</c:f>
+              <c:f>Cases!$B$2:$B$24</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy\ h:mm</c:formatCode>
-                <c:ptCount val="22"/>
+                <c:ptCount val="23"/>
                 <c:pt idx="0">
                   <c:v>43889.416666666664</c:v>
                 </c:pt>
@@ -4518,16 +4596,19 @@
                 </c:pt>
                 <c:pt idx="21">
                   <c:v>43910</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>43911</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Cases!$P$2:$P$23</c:f>
+              <c:f>Cases!$P$2:$P$24</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="22"/>
+                <c:ptCount val="23"/>
                 <c:pt idx="4">
                   <c:v>1</c:v>
                 </c:pt>
@@ -4581,6 +4662,9 @@
                 </c:pt>
                 <c:pt idx="21">
                   <c:v>394</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>567</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4638,10 +4722,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Cases!$B$2:$B$23</c:f>
+              <c:f>Cases!$B$2:$B$24</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy\ h:mm</c:formatCode>
-                <c:ptCount val="22"/>
+                <c:ptCount val="23"/>
                 <c:pt idx="0">
                   <c:v>43889.416666666664</c:v>
                 </c:pt>
@@ -4707,16 +4791,19 @@
                 </c:pt>
                 <c:pt idx="21">
                   <c:v>43910</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>43911</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Cases!$H$2:$H$23</c:f>
+              <c:f>Cases!$H$2:$H$24</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="22"/>
+                <c:ptCount val="23"/>
                 <c:pt idx="2">
                   <c:v>1</c:v>
                 </c:pt>
@@ -4776,6 +4863,9 @@
                 </c:pt>
                 <c:pt idx="21">
                   <c:v>121</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>142</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4837,10 +4927,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Cases!$B$2:$B$23</c:f>
+              <c:f>Cases!$B$2:$B$24</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy\ h:mm</c:formatCode>
-                <c:ptCount val="22"/>
+                <c:ptCount val="23"/>
                 <c:pt idx="0">
                   <c:v>43889.416666666664</c:v>
                 </c:pt>
@@ -4906,16 +4996,19 @@
                 </c:pt>
                 <c:pt idx="21">
                   <c:v>43910</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>43911</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Cases!$R$2:$R$23</c:f>
+              <c:f>Cases!$R$2:$R$24</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="22"/>
+                <c:ptCount val="23"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -4981,6 +5074,9 @@
                 </c:pt>
                 <c:pt idx="21">
                   <c:v>266</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>308</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5038,10 +5134,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Cases!$B$2:$B$23</c:f>
+              <c:f>Cases!$B$2:$B$24</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy\ h:mm</c:formatCode>
-                <c:ptCount val="22"/>
+                <c:ptCount val="23"/>
                 <c:pt idx="0">
                   <c:v>43889.416666666664</c:v>
                 </c:pt>
@@ -5107,16 +5203,19 @@
                 </c:pt>
                 <c:pt idx="21">
                   <c:v>43910</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>43911</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Cases!$G$2:$G$23</c:f>
+              <c:f>Cases!$G$2:$G$24</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="22"/>
+                <c:ptCount val="23"/>
                 <c:pt idx="4">
                   <c:v>1</c:v>
                 </c:pt>
@@ -5170,6 +5269,9 @@
                 </c:pt>
                 <c:pt idx="21">
                   <c:v>192</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>254</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5228,10 +5330,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Cases!$B$2:$B$23</c:f>
+              <c:f>Cases!$B$2:$B$24</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy\ h:mm</c:formatCode>
-                <c:ptCount val="22"/>
+                <c:ptCount val="23"/>
                 <c:pt idx="0">
                   <c:v>43889.416666666664</c:v>
                 </c:pt>
@@ -5297,16 +5399,19 @@
                 </c:pt>
                 <c:pt idx="21">
                   <c:v>43910</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>43911</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Cases!$K$2:$K$23</c:f>
+              <c:f>Cases!$K$2:$K$24</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="22"/>
+                <c:ptCount val="23"/>
                 <c:pt idx="5">
                   <c:v>4</c:v>
                 </c:pt>
@@ -5357,6 +5462,9 @@
                 </c:pt>
                 <c:pt idx="21">
                   <c:v>131</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>165</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5418,10 +5526,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Cases!$B$2:$B$23</c:f>
+              <c:f>Cases!$B$2:$B$24</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy\ h:mm</c:formatCode>
-                <c:ptCount val="22"/>
+                <c:ptCount val="23"/>
                 <c:pt idx="0">
                   <c:v>43889.416666666664</c:v>
                 </c:pt>
@@ -5487,16 +5595,19 @@
                 </c:pt>
                 <c:pt idx="21">
                   <c:v>43910</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>43911</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Cases!$Q$2:$Q$23</c:f>
+              <c:f>Cases!$Q$2:$Q$24</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="22"/>
+                <c:ptCount val="23"/>
                 <c:pt idx="11">
                   <c:v>7</c:v>
                 </c:pt>
@@ -5529,6 +5640,9 @@
                 </c:pt>
                 <c:pt idx="21">
                   <c:v>180</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>188</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5589,10 +5703,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Cases!$B$2:$B$23</c:f>
+              <c:f>Cases!$B$2:$B$24</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy\ h:mm</c:formatCode>
-                <c:ptCount val="22"/>
+                <c:ptCount val="23"/>
                 <c:pt idx="0">
                   <c:v>43889.416666666664</c:v>
                 </c:pt>
@@ -5658,16 +5772,19 @@
                 </c:pt>
                 <c:pt idx="21">
                   <c:v>43910</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>43911</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Cases!$O$2:$O$23</c:f>
+              <c:f>Cases!$O$2:$O$24</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="22"/>
+                <c:ptCount val="23"/>
                 <c:pt idx="5">
                   <c:v>1</c:v>
                 </c:pt>
@@ -5718,6 +5835,9 @@
                 </c:pt>
                 <c:pt idx="21">
                   <c:v>146</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>187</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5778,10 +5898,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Cases!$B$2:$B$23</c:f>
+              <c:f>Cases!$B$2:$B$24</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy\ h:mm</c:formatCode>
-                <c:ptCount val="22"/>
+                <c:ptCount val="23"/>
                 <c:pt idx="0">
                   <c:v>43889.416666666664</c:v>
                 </c:pt>
@@ -5847,16 +5967,19 @@
                 </c:pt>
                 <c:pt idx="21">
                   <c:v>43910</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>43911</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Cases!$S$2:$S$23</c:f>
+              <c:f>Cases!$S$2:$S$24</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="22"/>
+                <c:ptCount val="23"/>
                 <c:pt idx="4">
                   <c:v>1</c:v>
                 </c:pt>
@@ -5910,6 +6033,9 @@
                 </c:pt>
                 <c:pt idx="21">
                   <c:v>149</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>187</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6423,7 +6549,7 @@
               <c:strCache>
                 <c:ptCount val="2"/>
                 <c:pt idx="1">
-                  <c:v>20.03.20</c:v>
+                  <c:v>21.03.20</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -6879,7 +7005,7 @@
           <c:strCache>
             <c:ptCount val="1"/>
             <c:pt idx="0">
-              <c:v>Infektionen gesamt und pro 1 Millionen Einwohner, 20.03.2020</c:v>
+              <c:v>Infektionen gesamt und pro 1 Millionen Einwohner, 21.03.2020</c:v>
             </c:pt>
           </c:strCache>
         </c:strRef>
@@ -7013,52 +7139,52 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
                 <c:pt idx="0">
-                  <c:v>2746</c:v>
+                  <c:v>3668</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2401</c:v>
+                  <c:v>2960</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>731</c:v>
+                  <c:v>866</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>192</c:v>
+                  <c:v>254</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>121</c:v>
+                  <c:v>142</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>586</c:v>
+                  <c:v>587</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>813</c:v>
+                  <c:v>1080</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>131</c:v>
+                  <c:v>165</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>803</c:v>
+                  <c:v>1023</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>3497</c:v>
+                  <c:v>3542</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>801</c:v>
+                  <c:v>938</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>146</c:v>
+                  <c:v>187</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>394</c:v>
+                  <c:v>567</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>180</c:v>
+                  <c:v>188</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>266</c:v>
+                  <c:v>308</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>149</c:v>
+                  <c:v>187</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -7178,52 +7304,52 @@
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="16"/>
                 <c:pt idx="0">
-                  <c:v>248.06901847418584</c:v>
+                  <c:v>331.36094674556216</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>183.60901450671807</c:v>
+                  <c:v>226.35680255722011</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>200.55970149253733</c:v>
+                  <c:v>237.59877085162424</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>76.436163860026284</c:v>
+                  <c:v>101.11867510649309</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>177.15959004392386</c:v>
+                  <c:v>207.90629575402636</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>318.27069302628718</c:v>
+                  <c:v>318.81381707582011</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>129.75198697692232</c:v>
+                  <c:v>172.36426314277506</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>81.381623905075486</c:v>
+                  <c:v>102.50357209417903</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>100.59631188614952</c:v>
+                  <c:v>128.15694527961514</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>195.00688686031663</c:v>
+                  <c:v>197.51626916192205</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>196.09283196239718</c:v>
+                  <c:v>229.63180571876225</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>147.40030287733467</c:v>
+                  <c:v>188.79353861686016</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>96.618357487922708</c:v>
+                  <c:v>139.04215404987863</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>81.510664311914141</c:v>
+                  <c:v>85.133360503554769</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>91.828632581903548</c:v>
+                  <c:v>106.32789035799358</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>69.525453781904716</c:v>
+                  <c:v>87.256777565209276</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -7345,52 +7471,52 @@
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="16"/>
                 <c:pt idx="0">
-                  <c:v>168.11773661996261</c:v>
+                  <c:v>200.7005608341203</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>168.11773661996261</c:v>
+                  <c:v>200.7005608341203</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>168.11773661996261</c:v>
+                  <c:v>200.7005608341203</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>168.11773661996261</c:v>
+                  <c:v>200.7005608341203</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>168.11773661996261</c:v>
+                  <c:v>200.7005608341203</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>168.11773661996261</c:v>
+                  <c:v>200.7005608341203</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>168.11773661996261</c:v>
+                  <c:v>200.7005608341203</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>168.11773661996261</c:v>
+                  <c:v>200.7005608341203</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>168.11773661996261</c:v>
+                  <c:v>200.7005608341203</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>168.11773661996261</c:v>
+                  <c:v>200.7005608341203</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>168.11773661996261</c:v>
+                  <c:v>200.7005608341203</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>168.11773661996261</c:v>
+                  <c:v>200.7005608341203</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>168.11773661996261</c:v>
+                  <c:v>200.7005608341203</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>168.11773661996261</c:v>
+                  <c:v>200.7005608341203</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>168.11773661996261</c:v>
+                  <c:v>200.7005608341203</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>168.11773661996261</c:v>
+                  <c:v>200.7005608341203</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -9563,8 +9689,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{BC3E90BD-768C-894C-8066-F63C881D4ADC}" name="Table5" displayName="Table5" ref="A1:W23" totalsRowShown="0" headerRowDxfId="29">
-  <autoFilter ref="A1:W23" xr:uid="{6D4C76C7-14AA-DE49-9FD4-833E447F2FCD}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{BC3E90BD-768C-894C-8066-F63C881D4ADC}" name="Table5" displayName="Table5" ref="A1:W24" totalsRowShown="0" headerRowDxfId="29">
+  <autoFilter ref="A1:W24" xr:uid="{6D4C76C7-14AA-DE49-9FD4-833E447F2FCD}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -9627,8 +9753,8 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{2B4CB1FE-2F78-654B-9A83-851BD72419FA}" name="Table7" displayName="Table7" ref="A1:S23" totalsRowShown="0" headerRowDxfId="22" dataDxfId="20" headerRowBorderDxfId="21" tableBorderDxfId="19">
-  <autoFilter ref="A1:S23" xr:uid="{5EC7B395-6250-0C4B-BF9E-DB8BEACEA0C0}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{2B4CB1FE-2F78-654B-9A83-851BD72419FA}" name="Table7" displayName="Table7" ref="A1:S24" totalsRowShown="0" headerRowDxfId="22" dataDxfId="20" headerRowBorderDxfId="21" tableBorderDxfId="19">
+  <autoFilter ref="A1:S24" xr:uid="{5EC7B395-6250-0C4B-BF9E-DB8BEACEA0C0}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -10045,7 +10171,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B05B1DF0-9508-684D-9C94-CA87D158EEEF}">
   <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
@@ -10128,7 +10254,7 @@
       </c>
       <c r="B2">
         <f>last_DE_Total</f>
-        <v>13957</v>
+        <v>16662</v>
       </c>
       <c r="D2" t="s">
         <v>56</v>
@@ -10151,7 +10277,7 @@
       </c>
       <c r="B4" s="13">
         <f xml:space="preserve"> LOG(B3/B2,2)</f>
-        <v>6.1628673162960297</v>
+        <v>5.9072946067841725</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -10160,7 +10286,7 @@
       </c>
       <c r="B5" s="34">
         <f>B4*E2</f>
-        <v>18.488601948888089</v>
+        <v>17.721883820352517</v>
       </c>
     </row>
   </sheetData>
@@ -10170,7 +10296,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FEA00A9F-6A15-E440-8C87-85055F8A0710}">
-  <dimension ref="A1:T20"/>
+  <dimension ref="A1:R20"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B1" sqref="B1:C17"/>
@@ -10180,46 +10306,43 @@
   <cols>
     <col min="1" max="1" width="23.5" style="49" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="20.5" style="49" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="42.5" style="49" bestFit="1" customWidth="1"/>
-    <col min="4" max="6" width="10.83203125" style="49"/>
-    <col min="7" max="7" width="13.1640625" style="49" bestFit="1" customWidth="1"/>
-    <col min="8" max="10" width="10.83203125" style="49"/>
-    <col min="11" max="11" width="13.1640625" style="49" bestFit="1" customWidth="1"/>
-    <col min="12" max="14" width="10.83203125" style="49"/>
+    <col min="3" max="4" width="10.83203125" style="49"/>
+    <col min="5" max="5" width="13.1640625" style="49" bestFit="1" customWidth="1"/>
+    <col min="6" max="8" width="10.83203125" style="49"/>
+    <col min="9" max="9" width="13.1640625" style="49" bestFit="1" customWidth="1"/>
+    <col min="10" max="12" width="10.83203125" style="49"/>
+    <col min="13" max="13" width="13.1640625" style="49" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.83203125" style="49"/>
     <col min="15" max="15" width="13.1640625" style="49" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="10.83203125" style="49"/>
-    <col min="17" max="17" width="13.1640625" style="49" bestFit="1" customWidth="1"/>
-    <col min="18" max="16384" width="10.83203125" style="49"/>
+    <col min="16" max="16384" width="10.83203125" style="49"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20">
-      <c r="A1" s="66" t="s">
-        <v>0</v>
+    <row r="1" spans="1:18">
+      <c r="A1" t="s">
+        <v>99</v>
       </c>
       <c r="B1" s="66">
-        <v>2746</v>
+        <v>3668</v>
       </c>
       <c r="C1" s="66">
-        <v>10</v>
-      </c>
-      <c r="D1" s="66"/>
+        <v>16</v>
+      </c>
+      <c r="D1"/>
       <c r="E1" s="66"/>
-      <c r="F1" s="66"/>
-      <c r="G1" s="66"/>
-      <c r="K1" s="66"/>
-      <c r="O1" s="66"/>
+      <c r="I1" s="66"/>
+      <c r="M1" s="66"/>
     </row>
-    <row r="2" spans="1:20">
-      <c r="A2" s="66" t="s">
+    <row r="2" spans="1:18">
+      <c r="A2" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="66">
-        <v>2401</v>
+        <v>2960</v>
       </c>
       <c r="C2" s="66">
-        <v>12</v>
-      </c>
-      <c r="D2" s="65"/>
+        <v>19</v>
+      </c>
+      <c r="D2"/>
       <c r="E2" s="65"/>
       <c r="F2" s="65"/>
       <c r="G2" s="65"/>
@@ -10234,278 +10357,240 @@
       <c r="P2" s="65"/>
       <c r="Q2" s="65"/>
       <c r="R2" s="65"/>
-      <c r="S2" s="65"/>
-      <c r="T2" s="65"/>
     </row>
-    <row r="3" spans="1:20">
-      <c r="A3" s="66" t="s">
+    <row r="3" spans="1:18">
+      <c r="A3" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="66">
-        <v>731</v>
+        <v>866</v>
       </c>
       <c r="C3" s="66">
-        <v>0</v>
-      </c>
-      <c r="D3" s="66"/>
-      <c r="E3" s="66"/>
-      <c r="F3" s="66"/>
+        <v>1</v>
+      </c>
+      <c r="D3"/>
     </row>
-    <row r="4" spans="1:20">
-      <c r="A4" s="66" t="s">
+    <row r="4" spans="1:18">
+      <c r="A4" t="s">
         <v>3</v>
       </c>
       <c r="B4" s="66">
-        <v>192</v>
+        <v>254</v>
       </c>
       <c r="C4" s="66">
         <v>0</v>
       </c>
-      <c r="D4" s="66"/>
-      <c r="E4" s="66"/>
-      <c r="F4" s="66"/>
-      <c r="Q4" s="66"/>
-      <c r="R4" s="66"/>
+      <c r="D4"/>
+      <c r="O4" s="66"/>
+      <c r="P4" s="66"/>
     </row>
-    <row r="5" spans="1:20">
-      <c r="A5" s="66" t="s">
+    <row r="5" spans="1:18">
+      <c r="A5" t="s">
         <v>4</v>
       </c>
       <c r="B5" s="66">
-        <v>121</v>
+        <v>142</v>
       </c>
       <c r="C5" s="66">
         <v>0</v>
       </c>
-      <c r="D5" s="66"/>
-      <c r="E5" s="66"/>
-      <c r="F5" s="66"/>
-      <c r="Q5" s="66"/>
-      <c r="R5" s="66"/>
+      <c r="D5"/>
+      <c r="O5" s="66"/>
+      <c r="P5" s="66"/>
     </row>
-    <row r="6" spans="1:20">
-      <c r="A6" s="66" t="s">
+    <row r="6" spans="1:18">
+      <c r="A6" t="s">
         <v>5</v>
       </c>
       <c r="B6" s="66">
-        <v>586</v>
+        <v>587</v>
       </c>
       <c r="C6" s="66">
         <v>0</v>
       </c>
-      <c r="D6" s="66"/>
-      <c r="E6" s="66"/>
-      <c r="F6" s="66"/>
-      <c r="Q6" s="66"/>
-      <c r="R6" s="66"/>
+      <c r="D6"/>
+      <c r="O6" s="66"/>
+      <c r="P6" s="66"/>
     </row>
-    <row r="7" spans="1:20">
-      <c r="A7" s="66" t="s">
+    <row r="7" spans="1:18">
+      <c r="A7" t="s">
         <v>6</v>
       </c>
       <c r="B7" s="66">
-        <v>813</v>
+        <v>1080</v>
       </c>
       <c r="C7" s="66">
-        <v>1</v>
-      </c>
-      <c r="D7" s="66"/>
-      <c r="E7" s="66"/>
-      <c r="F7" s="66"/>
-      <c r="Q7" s="66"/>
-      <c r="R7" s="66"/>
+        <v>2</v>
+      </c>
+      <c r="D7"/>
+      <c r="O7" s="66"/>
+      <c r="P7" s="66"/>
     </row>
-    <row r="8" spans="1:20">
-      <c r="A8" s="66" t="s">
-        <v>7</v>
+    <row r="8" spans="1:18">
+      <c r="A8" t="s">
+        <v>100</v>
       </c>
       <c r="B8" s="66">
-        <v>131</v>
+        <v>165</v>
       </c>
       <c r="C8" s="66">
         <v>0</v>
       </c>
-      <c r="D8" s="66"/>
-      <c r="E8" s="66"/>
-      <c r="F8" s="66"/>
-      <c r="Q8" s="66"/>
-      <c r="R8" s="66"/>
+      <c r="D8"/>
+      <c r="O8" s="66"/>
+      <c r="P8" s="66"/>
     </row>
-    <row r="9" spans="1:20">
-      <c r="A9" s="66" t="s">
+    <row r="9" spans="1:18">
+      <c r="A9" t="s">
         <v>8</v>
       </c>
       <c r="B9" s="66">
-        <v>803</v>
+        <v>1023</v>
       </c>
       <c r="C9" s="66">
         <v>0</v>
       </c>
-      <c r="D9" s="66"/>
-      <c r="E9" s="66"/>
-      <c r="F9" s="66"/>
-      <c r="Q9" s="66"/>
-      <c r="R9" s="66"/>
+      <c r="D9"/>
+      <c r="O9" s="66"/>
+      <c r="P9" s="66"/>
     </row>
-    <row r="10" spans="1:20">
-      <c r="A10" s="66" t="s">
-        <v>9</v>
+    <row r="10" spans="1:18">
+      <c r="A10" t="s">
+        <v>101</v>
       </c>
       <c r="B10" s="66">
-        <v>3497</v>
+        <v>3542</v>
       </c>
       <c r="C10" s="66">
         <v>6</v>
       </c>
-      <c r="D10" s="66"/>
-      <c r="E10" s="66"/>
-      <c r="F10" s="66"/>
-      <c r="Q10" s="66"/>
-      <c r="R10" s="66"/>
+      <c r="D10"/>
+      <c r="O10" s="66"/>
+      <c r="P10" s="66"/>
     </row>
-    <row r="11" spans="1:20">
-      <c r="A11" s="66" t="s">
-        <v>10</v>
+    <row r="11" spans="1:18">
+      <c r="A11" t="s">
+        <v>102</v>
       </c>
       <c r="B11" s="66">
-        <v>801</v>
+        <v>938</v>
       </c>
       <c r="C11" s="66">
         <v>1</v>
       </c>
-      <c r="D11" s="66"/>
-      <c r="E11" s="66"/>
-      <c r="F11" s="66"/>
-      <c r="Q11" s="66"/>
-      <c r="R11" s="66"/>
+      <c r="D11"/>
+      <c r="O11" s="66"/>
+      <c r="P11" s="66"/>
     </row>
-    <row r="12" spans="1:20">
-      <c r="A12" s="66" t="s">
+    <row r="12" spans="1:18">
+      <c r="A12" t="s">
         <v>11</v>
       </c>
       <c r="B12" s="66">
-        <v>146</v>
+        <v>187</v>
       </c>
       <c r="C12" s="66">
         <v>0</v>
       </c>
-      <c r="D12" s="66"/>
-      <c r="E12" s="66"/>
-      <c r="F12" s="66"/>
-      <c r="Q12" s="66"/>
-      <c r="R12" s="66"/>
+      <c r="D12"/>
+      <c r="O12" s="66"/>
+      <c r="P12" s="66"/>
     </row>
-    <row r="13" spans="1:20">
-      <c r="A13" s="66" t="s">
+    <row r="13" spans="1:18">
+      <c r="A13" t="s">
         <v>12</v>
       </c>
       <c r="B13" s="66">
-        <v>394</v>
+        <v>567</v>
       </c>
       <c r="C13" s="66">
         <v>0</v>
       </c>
-      <c r="D13" s="66"/>
-      <c r="E13" s="66"/>
-      <c r="F13" s="66"/>
-      <c r="Q13" s="66"/>
-      <c r="R13" s="66"/>
+      <c r="D13"/>
+      <c r="O13" s="66"/>
+      <c r="P13" s="66"/>
     </row>
-    <row r="14" spans="1:20">
-      <c r="A14" s="66" t="s">
+    <row r="14" spans="1:18">
+      <c r="A14" t="s">
         <v>13</v>
       </c>
       <c r="B14" s="66">
-        <v>180</v>
+        <v>188</v>
       </c>
       <c r="C14" s="66">
         <v>0</v>
       </c>
-      <c r="D14" s="66"/>
-      <c r="E14" s="66"/>
-      <c r="F14" s="66"/>
-      <c r="Q14" s="66"/>
-      <c r="R14" s="66"/>
+      <c r="D14"/>
+      <c r="O14" s="66"/>
+      <c r="P14" s="66"/>
     </row>
-    <row r="15" spans="1:20">
-      <c r="A15" s="66" t="s">
-        <v>14</v>
+    <row r="15" spans="1:18">
+      <c r="A15" t="s">
+        <v>103</v>
       </c>
       <c r="B15" s="66">
-        <v>266</v>
+        <v>308</v>
       </c>
       <c r="C15" s="66">
         <v>1</v>
       </c>
-      <c r="D15" s="66"/>
-      <c r="E15" s="66"/>
-      <c r="F15" s="66"/>
-      <c r="Q15" s="66"/>
-      <c r="R15" s="66"/>
+      <c r="D15"/>
+      <c r="O15" s="66"/>
+      <c r="P15" s="66"/>
     </row>
-    <row r="16" spans="1:20">
-      <c r="A16" s="66" t="s">
+    <row r="16" spans="1:18">
+      <c r="A16" t="s">
         <v>15</v>
       </c>
       <c r="B16" s="66">
-        <v>149</v>
+        <v>187</v>
       </c>
       <c r="C16" s="66">
         <v>0</v>
       </c>
-      <c r="D16" s="66"/>
-      <c r="E16" s="66"/>
-      <c r="F16" s="66"/>
-      <c r="Q16" s="66"/>
-      <c r="R16" s="66"/>
+      <c r="D16"/>
+      <c r="O16" s="66"/>
+      <c r="P16" s="66"/>
     </row>
-    <row r="17" spans="1:18">
-      <c r="A17" s="66" t="s">
+    <row r="17" spans="1:16">
+      <c r="A17" s="1" t="s">
         <v>16</v>
       </c>
       <c r="B17" s="66">
-        <v>13957</v>
+        <v>16662</v>
       </c>
       <c r="C17" s="66">
-        <v>31</v>
-      </c>
-      <c r="D17" s="66"/>
-      <c r="E17" s="66"/>
-      <c r="F17" s="66"/>
-      <c r="Q17" s="66"/>
-      <c r="R17" s="66"/>
+        <v>46</v>
+      </c>
+      <c r="D17"/>
+      <c r="O17" s="66"/>
+      <c r="P17" s="66"/>
     </row>
-    <row r="18" spans="1:18">
+    <row r="18" spans="1:16">
       <c r="A18" s="66"/>
       <c r="B18" s="66"/>
       <c r="C18" s="66"/>
       <c r="D18" s="66"/>
-      <c r="E18" s="66"/>
-      <c r="F18" s="66"/>
-      <c r="Q18" s="66"/>
-      <c r="R18" s="66"/>
+      <c r="O18" s="66"/>
+      <c r="P18" s="66"/>
     </row>
-    <row r="19" spans="1:18">
+    <row r="19" spans="1:16">
       <c r="A19" s="66"/>
       <c r="B19" s="66"/>
       <c r="C19" s="66"/>
       <c r="D19" s="66"/>
-      <c r="E19" s="66"/>
-      <c r="F19" s="66"/>
-      <c r="Q19" s="66"/>
-      <c r="R19" s="66"/>
+      <c r="O19" s="66"/>
+      <c r="P19" s="66"/>
     </row>
-    <row r="20" spans="1:18">
+    <row r="20" spans="1:16">
       <c r="A20" s="66"/>
       <c r="B20" s="66"/>
       <c r="C20" s="66"/>
       <c r="D20" s="66"/>
-      <c r="E20" s="66"/>
-      <c r="F20" s="66"/>
-      <c r="O20" s="94"/>
-      <c r="P20" s="94"/>
-      <c r="Q20" s="66"/>
-      <c r="R20" s="66"/>
+      <c r="M20" s="94"/>
+      <c r="N20" s="94"/>
+      <c r="O20" s="66"/>
+      <c r="P20" s="66"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -15442,11 +15527,11 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{233E67D7-4FF2-D745-A107-DDC4CB6E1273}">
-  <dimension ref="A1:Z23"/>
+  <dimension ref="A1:Z24"/>
   <sheetViews>
-    <sheetView zoomScale="125" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K32" sqref="K32"/>
+    <sheetView topLeftCell="C1" zoomScale="125" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I29" sqref="I29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -15545,7 +15630,7 @@
     <row r="2" spans="1:26">
       <c r="A2" s="69">
         <f t="shared" ref="A2:A17" si="0">A3-1</f>
-        <v>-21</v>
+        <v>-22</v>
       </c>
       <c r="B2" s="15">
         <v>43889.416666666664</v>
@@ -15580,13 +15665,17 @@
 ((T2-T1)/T1)/(B2-B1),
 "")</f>
         <v/>
+      </c>
+      <c r="W2" s="70">
+        <f>guide_start*EXP((Table5[[#This Row],[Date]]-date_last_DE_Total)*(LN(2)/guide_doubling))</f>
+        <v>56.879209835213864</v>
       </c>
       <c r="Z2" s="87"/>
     </row>
     <row r="3" spans="1:26">
       <c r="A3" s="69">
         <f t="shared" si="0"/>
-        <v>-20</v>
+        <v>-21</v>
       </c>
       <c r="B3" s="15">
         <v>43890.416666666664</v>
@@ -15625,20 +15714,20 @@
       </c>
       <c r="W3" s="70">
         <f>guide_start*EXP((Table5[[#This Row],[Date]]-date_last_DE_Total)*(LN(2)/guide_doubling))</f>
-        <v>75.631927159515868</v>
+        <v>71.663313772773421</v>
       </c>
       <c r="Y3" t="s">
         <v>93</v>
       </c>
       <c r="Z3" s="50">
         <f>last_DE_Total*0.5</f>
-        <v>6978.5</v>
+        <v>8331</v>
       </c>
     </row>
     <row r="4" spans="1:26">
       <c r="A4" s="69">
         <f t="shared" si="0"/>
-        <v>-19</v>
+        <v>-20</v>
       </c>
       <c r="B4" s="15">
         <v>43891.625</v>
@@ -15686,7 +15775,7 @@
       </c>
       <c r="W4" s="70">
         <f>guide_start*EXP((Table5[[#This Row],[Date]]-date_last_DE_Total)*(LN(2)/guide_doubling))</f>
-        <v>99.989261179746862</v>
+        <v>94.742552080142715</v>
       </c>
       <c r="Y4" t="s">
         <v>94</v>
@@ -15698,7 +15787,7 @@
     <row r="5" spans="1:26">
       <c r="A5" s="69">
         <f t="shared" si="0"/>
-        <v>-18</v>
+        <v>-19</v>
       </c>
       <c r="B5" s="15">
         <v>43892.625</v>
@@ -15749,13 +15838,13 @@
       </c>
       <c r="W5" s="70">
         <f>guide_start*EXP((Table5[[#This Row],[Date]]-date_last_DE_Total)*(LN(2)/guide_doubling))</f>
-        <v>125.97857492379933</v>
+        <v>119.36813568653308</v>
       </c>
     </row>
     <row r="6" spans="1:26">
       <c r="A6" s="69">
         <f t="shared" si="0"/>
-        <v>-17</v>
+        <v>-18</v>
       </c>
       <c r="B6" s="15">
         <v>43893.625</v>
@@ -15815,7 +15904,7 @@
       </c>
       <c r="W6" s="70">
         <f>guide_start*EXP((Table5[[#This Row],[Date]]-date_last_DE_Total)*(LN(2)/guide_doubling))</f>
-        <v>158.72305838225327</v>
+        <v>150.3944268381704</v>
       </c>
       <c r="Y6" t="s">
         <v>86</v>
@@ -15827,7 +15916,7 @@
     <row r="7" spans="1:26">
       <c r="A7" s="69">
         <f t="shared" si="0"/>
-        <v>-16</v>
+        <v>-17</v>
       </c>
       <c r="B7" s="15">
         <v>43894.625</v>
@@ -15893,13 +15982,13 @@
       </c>
       <c r="W7" s="70">
         <f>guide_start*EXP((Table5[[#This Row],[Date]]-date_last_DE_Total)*(LN(2)/guide_doubling))</f>
-        <v>199.97852235949375</v>
+        <v>189.48510416028546</v>
       </c>
     </row>
     <row r="8" spans="1:26">
       <c r="A8" s="69">
         <f t="shared" si="0"/>
-        <v>-15</v>
+        <v>-16</v>
       </c>
       <c r="B8" s="15">
         <v>43895.625</v>
@@ -15965,13 +16054,13 @@
       </c>
       <c r="W8" s="70">
         <f>guide_start*EXP((Table5[[#This Row],[Date]]-date_last_DE_Total)*(LN(2)/guide_doubling))</f>
-        <v>251.95714984759874</v>
+        <v>238.73627137306619</v>
       </c>
     </row>
     <row r="9" spans="1:26">
       <c r="A9" s="69">
         <f t="shared" si="0"/>
-        <v>-14</v>
+        <v>-15</v>
       </c>
       <c r="B9" s="15">
         <v>43896.625</v>
@@ -16038,13 +16127,13 @@
       </c>
       <c r="W9" s="70">
         <f>guide_start*EXP((Table5[[#This Row],[Date]]-date_last_DE_Total)*(LN(2)/guide_doubling))</f>
-        <v>317.44611676450643</v>
+        <v>300.78885367634092</v>
       </c>
     </row>
     <row r="10" spans="1:26">
       <c r="A10" s="69">
         <f t="shared" si="0"/>
-        <v>-13</v>
+        <v>-14</v>
       </c>
       <c r="B10" s="15">
         <v>43897.625</v>
@@ -16110,13 +16199,13 @@
       </c>
       <c r="W10" s="70">
         <f>guide_start*EXP((Table5[[#This Row],[Date]]-date_last_DE_Total)*(LN(2)/guide_doubling))</f>
-        <v>399.9570447189875</v>
+        <v>378.97020832057075</v>
       </c>
     </row>
     <row r="11" spans="1:26">
       <c r="A11" s="69">
         <f t="shared" si="0"/>
-        <v>-12</v>
+        <v>-13</v>
       </c>
       <c r="B11" s="15">
         <v>43898.625</v>
@@ -16182,13 +16271,13 @@
       </c>
       <c r="W11" s="70">
         <f>guide_start*EXP((Table5[[#This Row],[Date]]-date_last_DE_Total)*(LN(2)/guide_doubling))</f>
-        <v>503.91429969519737</v>
+        <v>477.47254274613243</v>
       </c>
     </row>
     <row r="12" spans="1:26">
       <c r="A12" s="69">
         <f t="shared" si="0"/>
-        <v>-11</v>
+        <v>-12</v>
       </c>
       <c r="B12" s="15">
         <v>43899.625</v>
@@ -16254,13 +16343,13 @@
       </c>
       <c r="W12" s="70">
         <f>guide_start*EXP((Table5[[#This Row],[Date]]-date_last_DE_Total)*(LN(2)/guide_doubling))</f>
-        <v>634.89223352901297</v>
+        <v>601.57770735268173</v>
       </c>
     </row>
     <row r="13" spans="1:26">
       <c r="A13" s="69">
         <f t="shared" si="0"/>
-        <v>-10</v>
+        <v>-11</v>
       </c>
       <c r="B13" s="15">
         <v>43900.625</v>
@@ -16329,13 +16418,13 @@
       </c>
       <c r="W13" s="70">
         <f>guide_start*EXP((Table5[[#This Row],[Date]]-date_last_DE_Total)*(LN(2)/guide_doubling))</f>
-        <v>799.91408943797478</v>
+        <v>757.94041664114161</v>
       </c>
     </row>
     <row r="14" spans="1:26">
       <c r="A14" s="69">
         <f t="shared" si="0"/>
-        <v>-9</v>
+        <v>-10</v>
       </c>
       <c r="B14" s="15">
         <v>43901.625</v>
@@ -16404,13 +16493,13 @@
       </c>
       <c r="W14" s="70">
         <f>guide_start*EXP((Table5[[#This Row],[Date]]-date_last_DE_Total)*(LN(2)/guide_doubling))</f>
-        <v>1007.8285993903947</v>
+        <v>954.94508549226452</v>
       </c>
     </row>
     <row r="15" spans="1:26">
       <c r="A15" s="69">
         <f t="shared" si="0"/>
-        <v>-8</v>
+        <v>-9</v>
       </c>
       <c r="B15" s="16">
         <v>43902.625</v>
@@ -16479,14 +16568,14 @@
       </c>
       <c r="W15" s="70">
         <f>guide_start*EXP((Table5[[#This Row],[Date]]-date_last_DE_Total)*(LN(2)/guide_doubling))</f>
-        <v>1269.7844670580257</v>
+        <v>1203.1554147053635</v>
       </c>
       <c r="X15" s="40"/>
     </row>
     <row r="16" spans="1:26">
       <c r="A16" s="69">
         <f t="shared" si="0"/>
-        <v>-7</v>
+        <v>-8</v>
       </c>
       <c r="B16" s="16">
         <v>43903.625</v>
@@ -16557,14 +16646,14 @@
       </c>
       <c r="W16" s="70">
         <f>guide_start*EXP((Table5[[#This Row],[Date]]-date_last_DE_Total)*(LN(2)/guide_doubling))</f>
-        <v>1599.8281788759496</v>
+        <v>1515.880833282283</v>
       </c>
       <c r="X16" s="40"/>
     </row>
     <row r="17" spans="1:23">
       <c r="A17" s="69">
         <f t="shared" si="0"/>
-        <v>-6</v>
+        <v>-7</v>
       </c>
       <c r="B17" s="16">
         <v>43904.625</v>
@@ -16633,13 +16722,13 @@
       </c>
       <c r="W17" s="70">
         <f>guide_start*EXP((Table5[[#This Row],[Date]]-date_last_DE_Total)*(LN(2)/guide_doubling))</f>
-        <v>2015.6571987807893</v>
+        <v>1909.890170984529</v>
       </c>
     </row>
     <row r="18" spans="1:23">
       <c r="A18" s="69">
         <f>A19-1</f>
-        <v>-5</v>
+        <v>-6</v>
       </c>
       <c r="B18" s="37">
         <v>43905.625</v>
@@ -16708,13 +16797,13 @@
       </c>
       <c r="W18" s="70">
         <f>guide_start*EXP((Table5[[#This Row],[Date]]-date_last_DE_Total)*(LN(2)/guide_doubling))</f>
-        <v>2539.5689341160519</v>
+        <v>2406.3108294107265</v>
       </c>
     </row>
     <row r="19" spans="1:23">
       <c r="A19" s="69">
         <f>A20-1</f>
-        <v>-4</v>
+        <v>-5</v>
       </c>
       <c r="B19" s="37">
         <v>43906.625</v>
@@ -16783,13 +16872,13 @@
       </c>
       <c r="W19" s="70">
         <f>guide_start*EXP((Table5[[#This Row],[Date]]-date_last_DE_Total)*(LN(2)/guide_doubling))</f>
-        <v>3199.6563577518991</v>
+        <v>3031.7616665645664</v>
       </c>
     </row>
     <row r="20" spans="1:23">
       <c r="A20" s="69">
         <f>A21-1</f>
-        <v>-3</v>
+        <v>-4</v>
       </c>
       <c r="B20" s="37">
         <v>43907.625</v>
@@ -16858,13 +16947,13 @@
       </c>
       <c r="W20" s="70">
         <f>guide_start*EXP((Table5[[#This Row],[Date]]-date_last_DE_Total)*(LN(2)/guide_doubling))</f>
-        <v>4031.314397561579</v>
+        <v>3819.7803419690581</v>
       </c>
     </row>
     <row r="21" spans="1:23">
       <c r="A21" s="69">
         <f>A22-1</f>
-        <v>-2</v>
+        <v>-3</v>
       </c>
       <c r="B21" s="37">
         <v>43908</v>
@@ -16933,13 +17022,13 @@
       </c>
       <c r="W21" s="70">
         <f>guide_start*EXP((Table5[[#This Row],[Date]]-date_last_DE_Total)*(LN(2)/guide_doubling))</f>
-        <v>4396.179523345686</v>
+        <v>4165.5</v>
       </c>
     </row>
     <row r="22" spans="1:23">
       <c r="A22" s="69">
         <f>A23-1</f>
-        <v>-1</v>
+        <v>-2</v>
       </c>
       <c r="B22" s="89">
         <v>43909</v>
@@ -17010,12 +17099,13 @@
       </c>
       <c r="W22" s="88">
         <f>guide_start*EXP(Table5[[#This Row],['#]]*(LN(2)/guide_doubling))</f>
-        <v>5538.8391205800408</v>
+        <v>5248.2011333370947</v>
       </c>
     </row>
     <row r="23" spans="1:23">
-      <c r="A23" s="95">
-        <v>0</v>
+      <c r="A23" s="69">
+        <f>A24-1</f>
+        <v>-1</v>
       </c>
       <c r="B23" s="37">
         <v>43910</v>
@@ -17086,7 +17176,83 @@
       </c>
       <c r="W23" s="88">
         <f>guide_start*EXP(Table5[[#This Row],['#]]*(LN(2)/guide_doubling))</f>
-        <v>6978.5</v>
+        <v>6612.3190819735355</v>
+      </c>
+    </row>
+    <row r="24" spans="1:23">
+      <c r="A24" s="69">
+        <v>0</v>
+      </c>
+      <c r="B24" s="37">
+        <v>43911</v>
+      </c>
+      <c r="C24" s="72" t="s">
+        <v>42</v>
+      </c>
+      <c r="D24" s="66">
+        <v>3668</v>
+      </c>
+      <c r="E24" s="66">
+        <v>2960</v>
+      </c>
+      <c r="F24" s="66">
+        <v>866</v>
+      </c>
+      <c r="G24" s="66">
+        <v>254</v>
+      </c>
+      <c r="H24" s="66">
+        <v>142</v>
+      </c>
+      <c r="I24" s="66">
+        <v>587</v>
+      </c>
+      <c r="J24" s="66">
+        <v>1080</v>
+      </c>
+      <c r="K24" s="66">
+        <v>165</v>
+      </c>
+      <c r="L24" s="66">
+        <v>1023</v>
+      </c>
+      <c r="M24" s="66">
+        <v>3542</v>
+      </c>
+      <c r="N24" s="66">
+        <v>938</v>
+      </c>
+      <c r="O24" s="66">
+        <v>187</v>
+      </c>
+      <c r="P24" s="66">
+        <v>567</v>
+      </c>
+      <c r="Q24" s="66">
+        <v>188</v>
+      </c>
+      <c r="R24" s="66">
+        <v>308</v>
+      </c>
+      <c r="S24" s="66">
+        <v>187</v>
+      </c>
+      <c r="T24" s="66">
+        <v>16662</v>
+      </c>
+      <c r="U24" s="38">
+        <f>IF(ISNUMBER(T23),T24-T23,"")</f>
+        <v>2705</v>
+      </c>
+      <c r="V24" s="39">
+        <f>IF(ISNUMBER(T23),
+((T24-T23)/T23)/(B24-B23),
+"")</f>
+        <v>0.19380955792792148</v>
+      </c>
+      <c r="W24" s="88">
+        <f>guide_start*EXP(Table5[[#This Row],['#]]*(LN(2)/guide_doubling))</f>
+        <v>8331</v>
       </c>
     </row>
   </sheetData>
@@ -17101,11 +17267,11 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D35575D0-0A0E-6E43-9D76-74E38D2BC332}">
-  <dimension ref="A1:V23"/>
+  <dimension ref="A1:V24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K27" sqref="K27"/>
+      <selection pane="bottomLeft" activeCell="S23" sqref="S23:S24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -17192,7 +17358,7 @@
     <row r="2" spans="1:22">
       <c r="A2" s="29">
         <f>Cases!A2</f>
-        <v>-21</v>
+        <v>-22</v>
       </c>
       <c r="B2" s="21">
         <f>Cases!B2</f>
@@ -17310,7 +17476,7 @@
     <row r="3" spans="1:22">
       <c r="A3" s="30">
         <f>Cases!A3</f>
-        <v>-20</v>
+        <v>-21</v>
       </c>
       <c r="B3" s="21">
         <f>Cases!B3</f>
@@ -17422,7 +17588,7 @@
     <row r="4" spans="1:22">
       <c r="A4" s="30">
         <f>Cases!A4</f>
-        <v>-19</v>
+        <v>-20</v>
       </c>
       <c r="B4" s="21">
         <f>Cases!B4</f>
@@ -17534,7 +17700,7 @@
     <row r="5" spans="1:22">
       <c r="A5" s="30">
         <f>Cases!A5</f>
-        <v>-18</v>
+        <v>-19</v>
       </c>
       <c r="B5" s="21">
         <f>Cases!B5</f>
@@ -17646,7 +17812,7 @@
     <row r="6" spans="1:22">
       <c r="A6" s="30">
         <f>Cases!A6</f>
-        <v>-17</v>
+        <v>-18</v>
       </c>
       <c r="B6" s="21">
         <f>Cases!B6</f>
@@ -17758,7 +17924,7 @@
     <row r="7" spans="1:22">
       <c r="A7" s="30">
         <f>Cases!A7</f>
-        <v>-16</v>
+        <v>-17</v>
       </c>
       <c r="B7" s="21">
         <f>Cases!B7</f>
@@ -17870,7 +18036,7 @@
     <row r="8" spans="1:22">
       <c r="A8" s="30">
         <f>Cases!A8</f>
-        <v>-15</v>
+        <v>-16</v>
       </c>
       <c r="B8" s="21">
         <f>Cases!B8</f>
@@ -17982,7 +18148,7 @@
     <row r="9" spans="1:22">
       <c r="A9" s="30">
         <f>Cases!A9</f>
-        <v>-14</v>
+        <v>-15</v>
       </c>
       <c r="B9" s="21">
         <f>Cases!B9</f>
@@ -18094,7 +18260,7 @@
     <row r="10" spans="1:22">
       <c r="A10" s="30">
         <f>Cases!A10</f>
-        <v>-13</v>
+        <v>-14</v>
       </c>
       <c r="B10" s="21">
         <f>Cases!B10</f>
@@ -18206,7 +18372,7 @@
     <row r="11" spans="1:22">
       <c r="A11" s="30">
         <f>Cases!A11</f>
-        <v>-12</v>
+        <v>-13</v>
       </c>
       <c r="B11" s="21">
         <f>Cases!B11</f>
@@ -18318,7 +18484,7 @@
     <row r="12" spans="1:22">
       <c r="A12" s="30">
         <f>Cases!A12</f>
-        <v>-11</v>
+        <v>-12</v>
       </c>
       <c r="B12" s="21">
         <f>Cases!B12</f>
@@ -18430,7 +18596,7 @@
     <row r="13" spans="1:22">
       <c r="A13" s="30">
         <f>Cases!A13</f>
-        <v>-10</v>
+        <v>-11</v>
       </c>
       <c r="B13" s="21">
         <f>Cases!B13</f>
@@ -18542,7 +18708,7 @@
     <row r="14" spans="1:22">
       <c r="A14" s="30">
         <f>Cases!A14</f>
-        <v>-9</v>
+        <v>-10</v>
       </c>
       <c r="B14" s="21">
         <f>Cases!B14</f>
@@ -18654,7 +18820,7 @@
     <row r="15" spans="1:22">
       <c r="A15" s="41">
         <f>Cases!A15</f>
-        <v>-8</v>
+        <v>-9</v>
       </c>
       <c r="B15" s="42">
         <f>Cases!B15</f>
@@ -18766,7 +18932,7 @@
     <row r="16" spans="1:22">
       <c r="A16" s="29">
         <f>Cases!A16</f>
-        <v>-7</v>
+        <v>-8</v>
       </c>
       <c r="B16" s="21">
         <f>Cases!B16</f>
@@ -18878,7 +19044,7 @@
     <row r="17" spans="1:19">
       <c r="A17" s="41">
         <f>Cases!A17</f>
-        <v>-6</v>
+        <v>-7</v>
       </c>
       <c r="B17" s="42">
         <f>Cases!B17</f>
@@ -18990,7 +19156,7 @@
     <row r="18" spans="1:19">
       <c r="A18" s="41">
         <f>Cases!A18</f>
-        <v>-5</v>
+        <v>-6</v>
       </c>
       <c r="B18" s="42">
         <f>Cases!B18</f>
@@ -19102,7 +19268,7 @@
     <row r="19" spans="1:19">
       <c r="A19" s="41">
         <f>Cases!A19</f>
-        <v>-4</v>
+        <v>-5</v>
       </c>
       <c r="B19" s="42">
         <f>Cases!B19</f>
@@ -19214,7 +19380,7 @@
     <row r="20" spans="1:19">
       <c r="A20" s="41">
         <f>Cases!A20</f>
-        <v>-3</v>
+        <v>-4</v>
       </c>
       <c r="B20" s="42">
         <f>Cases!B20</f>
@@ -19326,7 +19492,7 @@
     <row r="21" spans="1:19">
       <c r="A21" s="41">
         <f>Cases!A21</f>
-        <v>-2</v>
+        <v>-3</v>
       </c>
       <c r="B21" s="42">
         <f>Cases!B21</f>
@@ -19438,7 +19604,7 @@
     <row r="22" spans="1:19">
       <c r="A22" s="30">
         <f>Cases!A22</f>
-        <v>-1</v>
+        <v>-2</v>
       </c>
       <c r="B22" s="93">
         <f>Cases!B22</f>
@@ -19550,7 +19716,7 @@
     <row r="23" spans="1:19">
       <c r="A23" s="30">
         <f>Cases!A23</f>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="B23" s="93">
         <f>Cases!B23</f>
@@ -19659,8 +19825,120 @@
         <v>0.26893353941267389</v>
       </c>
     </row>
+    <row r="24" spans="1:19">
+      <c r="A24" s="30">
+        <f>Cases!A24</f>
+        <v>0</v>
+      </c>
+      <c r="B24" s="93">
+        <f>Cases!B24</f>
+        <v>43911</v>
+      </c>
+      <c r="C24" s="22">
+        <f>IF(AND(ISNUMBER(Cases!D23),Cases!D23&gt;min_number),
+((Cases!D24-Cases!D23)/Cases!D23)/(Cases!$B24-Cases!$B23),
+"")</f>
+        <v>0.33576110706482154</v>
+      </c>
+      <c r="D24" s="22">
+        <f>IF(AND(ISNUMBER(Cases!E23),Cases!E23&gt;min_number),
+((Cases!E24-Cases!E23)/Cases!E23)/(Cases!$B24-Cases!$B23),
+"")</f>
+        <v>0.23281965847563516</v>
+      </c>
+      <c r="E24" s="22">
+        <f>IF(AND(ISNUMBER(Cases!F23),Cases!F23&gt;min_number),
+((Cases!F24-Cases!F23)/Cases!F23)/(Cases!$B24-Cases!$B23),
+"")</f>
+        <v>0.18467852257181944</v>
+      </c>
+      <c r="F24" s="22">
+        <f>IF(AND(ISNUMBER(Cases!G23),Cases!G23&gt;min_number),
+((Cases!G24-Cases!G23)/Cases!G23)/(Cases!$B24-Cases!$B23),
+"")</f>
+        <v>0.32291666666666669</v>
+      </c>
+      <c r="G24" s="22">
+        <f>IF(AND(ISNUMBER(Cases!H23),Cases!H23&gt;min_number),
+((Cases!H24-Cases!H23)/Cases!H23)/(Cases!$B24-Cases!$B23),
+"")</f>
+        <v>0.17355371900826447</v>
+      </c>
+      <c r="H24" s="22">
+        <f>IF(AND(ISNUMBER(Cases!I23),Cases!I23&gt;min_number),
+((Cases!I24-Cases!I23)/Cases!I23)/(Cases!$B24-Cases!$B23),
+"")</f>
+        <v>1.7064846416382253E-3</v>
+      </c>
+      <c r="I24" s="22">
+        <f>IF(AND(ISNUMBER(Cases!J23),Cases!J23&gt;min_number),
+((Cases!J24-Cases!J23)/Cases!J23)/(Cases!$B24-Cases!$B23),
+"")</f>
+        <v>0.32841328413284132</v>
+      </c>
+      <c r="J24" s="22">
+        <f>IF(AND(ISNUMBER(Cases!K23),Cases!K23&gt;min_number),
+((Cases!K24-Cases!K23)/Cases!K23)/(Cases!$B24-Cases!$B23),
+"")</f>
+        <v>0.25954198473282442</v>
+      </c>
+      <c r="K24" s="22">
+        <f>IF(AND(ISNUMBER(Cases!L23),Cases!L23&gt;min_number),
+((Cases!L24-Cases!L23)/Cases!L23)/(Cases!$B24-Cases!$B23),
+"")</f>
+        <v>0.27397260273972601</v>
+      </c>
+      <c r="L24" s="22">
+        <f>IF(AND(ISNUMBER(Cases!M23),Cases!M23&gt;min_number),
+((Cases!M24-Cases!M23)/Cases!M23)/(Cases!$B24-Cases!$B23),
+"")</f>
+        <v>1.2868172719473835E-2</v>
+      </c>
+      <c r="M24" s="22">
+        <f>IF(AND(ISNUMBER(Cases!N23),Cases!N23&gt;min_number),
+((Cases!N24-Cases!N23)/Cases!N23)/(Cases!$B24-Cases!$B23),
+"")</f>
+        <v>0.17103620474406991</v>
+      </c>
+      <c r="N24" s="22">
+        <f>IF(AND(ISNUMBER(Cases!O23),Cases!O23&gt;min_number),
+((Cases!O24-Cases!O23)/Cases!O23)/(Cases!$B24-Cases!$B23),
+"")</f>
+        <v>0.28082191780821919</v>
+      </c>
+      <c r="O24" s="22">
+        <f>IF(AND(ISNUMBER(Cases!P23),Cases!P23&gt;min_number),
+((Cases!P24-Cases!P23)/Cases!P23)/(Cases!$B24-Cases!$B23),
+"")</f>
+        <v>0.43908629441624364</v>
+      </c>
+      <c r="P24" s="22">
+        <f>IF(AND(ISNUMBER(Cases!Q23),Cases!Q23&gt;min_number),
+((Cases!Q24-Cases!Q23)/Cases!Q23)/(Cases!$B24-Cases!$B23),
+"")</f>
+        <v>4.4444444444444446E-2</v>
+      </c>
+      <c r="Q24" s="22">
+        <f>IF(AND(ISNUMBER(Cases!R23),Cases!R23&gt;min_number),
+((Cases!R24-Cases!R23)/Cases!R23)/(Cases!$B24-Cases!$B23),
+"")</f>
+        <v>0.15789473684210525</v>
+      </c>
+      <c r="R24" s="22">
+        <f>IF(AND(ISNUMBER(Cases!S23),Cases!S23&gt;min_number),
+((Cases!S24-Cases!S23)/Cases!S23)/(Cases!$B24-Cases!$B23),
+"")</f>
+        <v>0.25503355704697989</v>
+      </c>
+      <c r="S24" s="44">
+        <f>IF(AND(ISNUMBER(Cases!T23),Cases!T23&gt;min_number),
+((Cases!T24-Cases!T23)/Cases!T23)/(Cases!$B24-Cases!$B23),
+"")</f>
+        <v>0.19380955792792148</v>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="C2:S23">
+  <conditionalFormatting sqref="C2:S24">
     <cfRule type="colorScale" priority="6">
       <colorScale>
         <cfvo type="min"/>
@@ -19681,9 +19959,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C283F65E-4645-8A47-BFE2-5D2317004015}">
   <dimension ref="A1:W21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B20" sqref="B5:B20"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
@@ -19731,7 +20007,7 @@
       </c>
       <c r="I2" s="64" t="str">
         <f>"Infektionen gesamt und pro 1 Millionen Einwohner, "&amp;TEXT(C3,"TT.MM.JJJJ")</f>
-        <v>Infektionen gesamt und pro 1 Millionen Einwohner, 20.03.2020</v>
+        <v>Infektionen gesamt und pro 1 Millionen Einwohner, 21.03.2020</v>
       </c>
       <c r="U2" s="34"/>
       <c r="V2" s="12"/>
@@ -19740,7 +20016,7 @@
     <row r="3" spans="1:23">
       <c r="C3" s="63">
         <f>LOOKUP(2,1/(ISNUMBER(Cases!B2:B9998)),Cases!B2:B9998)</f>
-        <v>43910</v>
+        <v>43911</v>
       </c>
       <c r="U3" s="34"/>
       <c r="V3" s="12"/>
@@ -19774,15 +20050,15 @@
       </c>
       <c r="C5" s="51">
         <f>LOOKUP(2,1/(ISNUMBER(Cases!D2:D9998)),Cases!D2:D9998)</f>
-        <v>2746</v>
+        <v>3668</v>
       </c>
       <c r="D5" s="77">
         <f>last_BW/pop_BW*per_pop_scale</f>
-        <v>248.06901847418584</v>
+        <v>331.36094674556216</v>
       </c>
       <c r="E5" s="34">
         <f>$D$21</f>
-        <v>168.11773661996261</v>
+        <v>200.7005608341203</v>
       </c>
     </row>
     <row r="6" spans="1:23">
@@ -19794,15 +20070,15 @@
       </c>
       <c r="C6" s="51">
         <f>LOOKUP(2,1/(ISNUMBER(Cases!E2:E9998)),Cases!E2:E9998)</f>
-        <v>2401</v>
+        <v>2960</v>
       </c>
       <c r="D6" s="77">
         <f>last_BY/pop_BY*per_pop_scale</f>
-        <v>183.60901450671807</v>
+        <v>226.35680255722011</v>
       </c>
       <c r="E6" s="34">
         <f t="shared" ref="E6:E20" si="0">$D$21</f>
-        <v>168.11773661996261</v>
+        <v>200.7005608341203</v>
       </c>
     </row>
     <row r="7" spans="1:23">
@@ -19814,15 +20090,15 @@
       </c>
       <c r="C7" s="51">
         <f>LOOKUP(2,1/(ISNUMBER(Cases!F2:F9998)),Cases!F2:F9998)</f>
-        <v>731</v>
+        <v>866</v>
       </c>
       <c r="D7" s="77">
         <f>last_BE/pop_BE*per_pop_scale</f>
-        <v>200.55970149253733</v>
+        <v>237.59877085162424</v>
       </c>
       <c r="E7" s="34">
         <f t="shared" si="0"/>
-        <v>168.11773661996261</v>
+        <v>200.7005608341203</v>
       </c>
     </row>
     <row r="8" spans="1:23">
@@ -19834,15 +20110,15 @@
       </c>
       <c r="C8" s="51">
         <f>LOOKUP(2,1/(ISNUMBER(Cases!G2:G9998)),Cases!G2:G9998)</f>
-        <v>192</v>
+        <v>254</v>
       </c>
       <c r="D8" s="77">
         <f>last_BB/pop_BB*per_pop_scale</f>
-        <v>76.436163860026284</v>
+        <v>101.11867510649309</v>
       </c>
       <c r="E8" s="34">
         <f t="shared" si="0"/>
-        <v>168.11773661996261</v>
+        <v>200.7005608341203</v>
       </c>
     </row>
     <row r="9" spans="1:23">
@@ -19854,15 +20130,15 @@
       </c>
       <c r="C9" s="51">
         <f>LOOKUP(2,1/(ISNUMBER(Cases!H2:H9998)),Cases!H2:H9998)</f>
-        <v>121</v>
+        <v>142</v>
       </c>
       <c r="D9" s="77">
         <f>last_HB/pop_HB*per_pop_scale</f>
-        <v>177.15959004392386</v>
+        <v>207.90629575402636</v>
       </c>
       <c r="E9" s="34">
         <f t="shared" si="0"/>
-        <v>168.11773661996261</v>
+        <v>200.7005608341203</v>
       </c>
     </row>
     <row r="10" spans="1:23">
@@ -19874,15 +20150,15 @@
       </c>
       <c r="C10" s="51">
         <f>LOOKUP(2,1/(ISNUMBER(Cases!I2:I9998)),Cases!I2:I9998)</f>
-        <v>586</v>
+        <v>587</v>
       </c>
       <c r="D10" s="77">
         <f>last_HH/pop_HH*per_pop_scale</f>
-        <v>318.27069302628718</v>
+        <v>318.81381707582011</v>
       </c>
       <c r="E10" s="34">
         <f t="shared" si="0"/>
-        <v>168.11773661996261</v>
+        <v>200.7005608341203</v>
       </c>
     </row>
     <row r="11" spans="1:23">
@@ -19894,15 +20170,15 @@
       </c>
       <c r="C11" s="51">
         <f>LOOKUP(2,1/(ISNUMBER(Cases!J2:J9998)),Cases!J2:J9998)</f>
-        <v>813</v>
+        <v>1080</v>
       </c>
       <c r="D11" s="77">
         <f>last_HE/pop_HE*per_pop_scale</f>
-        <v>129.75198697692232</v>
+        <v>172.36426314277506</v>
       </c>
       <c r="E11" s="34">
         <f t="shared" si="0"/>
-        <v>168.11773661996261</v>
+        <v>200.7005608341203</v>
       </c>
     </row>
     <row r="12" spans="1:23" ht="34">
@@ -19914,15 +20190,15 @@
       </c>
       <c r="C12" s="51">
         <f>LOOKUP(2,1/(ISNUMBER(Cases!K2:K9998)),Cases!K2:K9998)</f>
-        <v>131</v>
+        <v>165</v>
       </c>
       <c r="D12" s="77">
         <f>last_MV/pop_MV*per_pop_scale</f>
-        <v>81.381623905075486</v>
+        <v>102.50357209417903</v>
       </c>
       <c r="E12" s="34">
         <f t="shared" si="0"/>
-        <v>168.11773661996261</v>
+        <v>200.7005608341203</v>
       </c>
     </row>
     <row r="13" spans="1:23">
@@ -19934,15 +20210,15 @@
       </c>
       <c r="C13" s="51">
         <f>LOOKUP(2,1/(ISNUMBER(Cases!L2:L9998)),Cases!L2:L9998)</f>
-        <v>803</v>
+        <v>1023</v>
       </c>
       <c r="D13" s="77">
         <f>last_NI/pop_NI*per_pop_scale</f>
-        <v>100.59631188614952</v>
+        <v>128.15694527961514</v>
       </c>
       <c r="E13" s="34">
         <f t="shared" si="0"/>
-        <v>168.11773661996261</v>
+        <v>200.7005608341203</v>
       </c>
     </row>
     <row r="14" spans="1:23" ht="34">
@@ -19954,15 +20230,15 @@
       </c>
       <c r="C14" s="51">
         <f>LOOKUP(2,1/(ISNUMBER(Cases!M2:M9998)),Cases!M2:M9998)</f>
-        <v>3497</v>
+        <v>3542</v>
       </c>
       <c r="D14" s="77">
         <f>last_NW/pop_NW*per_pop_scale</f>
-        <v>195.00688686031663</v>
+        <v>197.51626916192205</v>
       </c>
       <c r="E14" s="34">
         <f t="shared" si="0"/>
-        <v>168.11773661996261</v>
+        <v>200.7005608341203</v>
       </c>
     </row>
     <row r="15" spans="1:23" ht="34">
@@ -19974,15 +20250,15 @@
       </c>
       <c r="C15" s="51">
         <f>LOOKUP(2,1/(ISNUMBER(Cases!N2:N9998)),Cases!N2:N9998)</f>
-        <v>801</v>
+        <v>938</v>
       </c>
       <c r="D15" s="77">
         <f>last_RP/pop_RP*per_pop_scale</f>
-        <v>196.09283196239718</v>
+        <v>229.63180571876225</v>
       </c>
       <c r="E15" s="34">
         <f t="shared" si="0"/>
-        <v>168.11773661996261</v>
+        <v>200.7005608341203</v>
       </c>
     </row>
     <row r="16" spans="1:23">
@@ -19994,15 +20270,15 @@
       </c>
       <c r="C16" s="51">
         <f>LOOKUP(2,1/(ISNUMBER(Cases!O2:O9998)),Cases!O2:O9998)</f>
-        <v>146</v>
+        <v>187</v>
       </c>
       <c r="D16" s="77">
         <f>last_SL/pop_SL*per_pop_scale</f>
-        <v>147.40030287733467</v>
+        <v>188.79353861686016</v>
       </c>
       <c r="E16" s="34">
         <f t="shared" si="0"/>
-        <v>168.11773661996261</v>
+        <v>200.7005608341203</v>
       </c>
       <c r="F16" s="56"/>
       <c r="G16" s="56"/>
@@ -20021,15 +20297,15 @@
       </c>
       <c r="C17" s="51">
         <f>LOOKUP(2,1/(ISNUMBER(Cases!P2:P9998)),Cases!P2:P9998)</f>
-        <v>394</v>
+        <v>567</v>
       </c>
       <c r="D17" s="77">
         <f>last_SN/pop_SN*per_pop_scale</f>
-        <v>96.618357487922708</v>
+        <v>139.04215404987863</v>
       </c>
       <c r="E17" s="34">
         <f t="shared" si="0"/>
-        <v>168.11773661996261</v>
+        <v>200.7005608341203</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="34">
@@ -20041,15 +20317,15 @@
       </c>
       <c r="C18" s="51">
         <f>LOOKUP(2,1/(ISNUMBER(Cases!Q2:Q9998)),Cases!Q2:Q9998)</f>
-        <v>180</v>
+        <v>188</v>
       </c>
       <c r="D18" s="77">
         <f>last_ST/pop_ST*per_pop_scale</f>
-        <v>81.510664311914141</v>
+        <v>85.133360503554769</v>
       </c>
       <c r="E18" s="34">
         <f t="shared" si="0"/>
-        <v>168.11773661996261</v>
+        <v>200.7005608341203</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="34">
@@ -20061,15 +20337,15 @@
       </c>
       <c r="C19" s="51">
         <f>LOOKUP(2,1/(ISNUMBER(Cases!R2:R9998)),Cases!R2:R9998)</f>
-        <v>266</v>
+        <v>308</v>
       </c>
       <c r="D19" s="77">
         <f>last_SH/pop_SH*per_pop_scale</f>
-        <v>91.828632581903548</v>
+        <v>106.32789035799358</v>
       </c>
       <c r="E19" s="34">
         <f t="shared" si="0"/>
-        <v>168.11773661996261</v>
+        <v>200.7005608341203</v>
       </c>
     </row>
     <row r="20" spans="1:5">
@@ -20081,15 +20357,15 @@
       </c>
       <c r="C20" s="51">
         <f>LOOKUP(2,1/(ISNUMBER(Cases!S2:S9998)),Cases!S2:S9998)</f>
-        <v>149</v>
+        <v>187</v>
       </c>
       <c r="D20" s="77">
         <f>last_TH/pop_TH*per_pop_scale</f>
-        <v>69.525453781904716</v>
+        <v>87.256777565209276</v>
       </c>
       <c r="E20" s="34">
         <f t="shared" si="0"/>
-        <v>168.11773661996261</v>
+        <v>200.7005608341203</v>
       </c>
     </row>
     <row r="21" spans="1:5">
@@ -20101,11 +20377,11 @@
       </c>
       <c r="C21" s="51">
         <f>LOOKUP(2,1/(ISNUMBER(Cases!T2:T9998)),Cases!T2:T9998)</f>
-        <v>13957</v>
+        <v>16662</v>
       </c>
       <c r="D21" s="77">
         <f>last_DE_Total/pop_DE_Total*per_pop_scale</f>
-        <v>168.11773661996261</v>
+        <v>200.7005608341203</v>
       </c>
     </row>
   </sheetData>
@@ -20136,10 +20412,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{960C88F9-5C4A-BD47-8A4B-0F1E4DF751E9}">
-  <dimension ref="A1:T45"/>
+  <dimension ref="A1:V45"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="V1" sqref="V1"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -20152,591 +20428,655 @@
     <col min="27" max="16384" width="10.83203125" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" s="17" customFormat="1" ht="142">
-      <c r="A1" s="111" t="s">
+    <row r="1" spans="1:22" s="17" customFormat="1" ht="142">
+      <c r="A1" s="110" t="s">
         <v>40</v>
       </c>
-      <c r="B1" s="112" t="s">
+      <c r="B1" s="111" t="s">
         <v>38</v>
       </c>
-      <c r="C1" s="113" t="s">
+      <c r="C1" s="112" t="s">
         <v>22</v>
       </c>
-      <c r="D1" s="113" t="s">
+      <c r="D1" s="112" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="113" t="s">
+      <c r="E1" s="112" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="113" t="s">
+      <c r="F1" s="112" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="113" t="s">
+      <c r="G1" s="112" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="113" t="s">
+      <c r="H1" s="112" t="s">
         <v>4</v>
       </c>
-      <c r="I1" s="113" t="s">
+      <c r="I1" s="112" t="s">
         <v>5</v>
       </c>
-      <c r="J1" s="113" t="s">
+      <c r="J1" s="112" t="s">
         <v>6</v>
       </c>
-      <c r="K1" s="113" t="s">
+      <c r="K1" s="112" t="s">
         <v>7</v>
       </c>
-      <c r="L1" s="113" t="s">
+      <c r="L1" s="112" t="s">
         <v>8</v>
       </c>
-      <c r="M1" s="113" t="s">
+      <c r="M1" s="112" t="s">
         <v>9</v>
       </c>
-      <c r="N1" s="113" t="s">
+      <c r="N1" s="112" t="s">
         <v>10</v>
       </c>
-      <c r="O1" s="113" t="s">
+      <c r="O1" s="112" t="s">
         <v>11</v>
       </c>
-      <c r="P1" s="113" t="s">
+      <c r="P1" s="112" t="s">
         <v>12</v>
       </c>
-      <c r="Q1" s="113" t="s">
+      <c r="Q1" s="112" t="s">
         <v>13</v>
       </c>
-      <c r="R1" s="113" t="s">
+      <c r="R1" s="112" t="s">
         <v>14</v>
       </c>
-      <c r="S1" s="113" t="s">
+      <c r="S1" s="112" t="s">
         <v>15</v>
       </c>
-      <c r="T1" s="112" t="s">
+      <c r="T1" s="111" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="2" spans="1:20">
-      <c r="A2" s="96">
+    <row r="2" spans="1:22">
+      <c r="A2" s="95">
         <v>10</v>
       </c>
-      <c r="B2" s="97">
+      <c r="B2" s="96">
         <v>43899.625</v>
       </c>
-      <c r="C2" s="98" t="s">
+      <c r="C2" s="97" t="s">
         <v>19</v>
       </c>
-      <c r="D2" s="99"/>
-      <c r="E2" s="99"/>
-      <c r="F2" s="99"/>
-      <c r="G2" s="99"/>
-      <c r="H2" s="99"/>
-      <c r="I2" s="99"/>
-      <c r="J2" s="99"/>
-      <c r="K2" s="99"/>
-      <c r="L2" s="99"/>
-      <c r="M2" s="99">
+      <c r="D2" s="98"/>
+      <c r="E2" s="98"/>
+      <c r="F2" s="98"/>
+      <c r="G2" s="98"/>
+      <c r="H2" s="98"/>
+      <c r="I2" s="98"/>
+      <c r="J2" s="98"/>
+      <c r="K2" s="98"/>
+      <c r="L2" s="98"/>
+      <c r="M2" s="98">
         <v>2</v>
       </c>
-      <c r="N2" s="99"/>
-      <c r="O2" s="99"/>
-      <c r="P2" s="99"/>
-      <c r="Q2" s="99"/>
-      <c r="R2" s="99"/>
-      <c r="S2" s="99"/>
-      <c r="T2" s="100">
+      <c r="N2" s="98"/>
+      <c r="O2" s="98"/>
+      <c r="P2" s="98"/>
+      <c r="Q2" s="98"/>
+      <c r="R2" s="98"/>
+      <c r="S2" s="98"/>
+      <c r="T2" s="99">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:20">
-      <c r="A3" s="96">
+    <row r="3" spans="1:22">
+      <c r="A3" s="95">
         <v>11</v>
       </c>
-      <c r="B3" s="97">
+      <c r="B3" s="96">
         <v>43900.625</v>
       </c>
-      <c r="C3" s="98" t="s">
+      <c r="C3" s="97" t="s">
         <v>19</v>
       </c>
-      <c r="D3" s="99"/>
-      <c r="E3" s="99"/>
-      <c r="F3" s="99"/>
-      <c r="G3" s="99"/>
-      <c r="H3" s="99"/>
-      <c r="I3" s="99"/>
-      <c r="J3" s="99"/>
-      <c r="K3" s="99"/>
-      <c r="L3" s="99"/>
-      <c r="M3" s="99">
+      <c r="D3" s="98"/>
+      <c r="E3" s="98"/>
+      <c r="F3" s="98"/>
+      <c r="G3" s="98"/>
+      <c r="H3" s="98"/>
+      <c r="I3" s="98"/>
+      <c r="J3" s="98"/>
+      <c r="K3" s="98"/>
+      <c r="L3" s="98"/>
+      <c r="M3" s="98">
         <v>2</v>
       </c>
-      <c r="N3" s="99"/>
-      <c r="O3" s="99"/>
-      <c r="P3" s="99"/>
-      <c r="Q3" s="99"/>
-      <c r="R3" s="99"/>
-      <c r="S3" s="99"/>
-      <c r="T3" s="100">
+      <c r="N3" s="98"/>
+      <c r="O3" s="98"/>
+      <c r="P3" s="98"/>
+      <c r="Q3" s="98"/>
+      <c r="R3" s="98"/>
+      <c r="S3" s="98"/>
+      <c r="T3" s="99">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:20">
-      <c r="A4" s="96">
+    <row r="4" spans="1:22">
+      <c r="A4" s="95">
         <v>12</v>
       </c>
-      <c r="B4" s="97">
+      <c r="B4" s="96">
         <v>43901.625</v>
       </c>
-      <c r="C4" s="98" t="s">
+      <c r="C4" s="97" t="s">
         <v>19</v>
       </c>
-      <c r="D4" s="99"/>
-      <c r="E4" s="99"/>
-      <c r="F4" s="99"/>
-      <c r="G4" s="99"/>
-      <c r="H4" s="99"/>
-      <c r="I4" s="99"/>
-      <c r="J4" s="99"/>
-      <c r="K4" s="99"/>
-      <c r="L4" s="99"/>
-      <c r="M4" s="99">
+      <c r="D4" s="98"/>
+      <c r="E4" s="98"/>
+      <c r="F4" s="98"/>
+      <c r="G4" s="98"/>
+      <c r="H4" s="98"/>
+      <c r="I4" s="98"/>
+      <c r="J4" s="98"/>
+      <c r="K4" s="98"/>
+      <c r="L4" s="98"/>
+      <c r="M4" s="98">
         <v>3</v>
       </c>
-      <c r="N4" s="99"/>
-      <c r="O4" s="99"/>
-      <c r="P4" s="99"/>
-      <c r="Q4" s="99"/>
-      <c r="R4" s="99"/>
-      <c r="S4" s="99"/>
-      <c r="T4" s="100">
+      <c r="N4" s="98"/>
+      <c r="O4" s="98"/>
+      <c r="P4" s="98"/>
+      <c r="Q4" s="98"/>
+      <c r="R4" s="98"/>
+      <c r="S4" s="98"/>
+      <c r="T4" s="99">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:20">
-      <c r="A5" s="96">
+    <row r="5" spans="1:22">
+      <c r="A5" s="95">
         <v>13</v>
       </c>
       <c r="B5" s="15">
         <v>43902.625</v>
       </c>
-      <c r="C5" s="101" t="s">
+      <c r="C5" s="100" t="s">
         <v>19</v>
       </c>
-      <c r="D5" s="99">
+      <c r="D5" s="98">
         <v>1</v>
       </c>
-      <c r="E5" s="99">
+      <c r="E5" s="98">
         <v>1</v>
       </c>
-      <c r="F5" s="99"/>
-      <c r="G5" s="99"/>
-      <c r="H5" s="99"/>
-      <c r="I5" s="99"/>
-      <c r="J5" s="99"/>
-      <c r="K5" s="99"/>
-      <c r="L5" s="99"/>
-      <c r="M5" s="99">
+      <c r="F5" s="98"/>
+      <c r="G5" s="98"/>
+      <c r="H5" s="98"/>
+      <c r="I5" s="98"/>
+      <c r="J5" s="98"/>
+      <c r="K5" s="98"/>
+      <c r="L5" s="98"/>
+      <c r="M5" s="98">
         <v>3</v>
       </c>
-      <c r="N5" s="99"/>
-      <c r="O5" s="99"/>
-      <c r="P5" s="99"/>
-      <c r="Q5" s="99"/>
-      <c r="R5" s="99"/>
-      <c r="S5" s="99"/>
-      <c r="T5" s="100">
+      <c r="N5" s="98"/>
+      <c r="O5" s="98"/>
+      <c r="P5" s="98"/>
+      <c r="Q5" s="98"/>
+      <c r="R5" s="98"/>
+      <c r="S5" s="98"/>
+      <c r="T5" s="99">
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:20">
-      <c r="A6" s="96">
+    <row r="6" spans="1:22">
+      <c r="A6" s="95">
         <v>14</v>
       </c>
-      <c r="B6" s="102">
+      <c r="B6" s="101">
         <v>43903.625</v>
       </c>
-      <c r="C6" s="101" t="s">
+      <c r="C6" s="100" t="s">
         <v>19</v>
       </c>
-      <c r="D6" s="103">
+      <c r="D6" s="102">
         <v>1</v>
       </c>
-      <c r="E6" s="103">
+      <c r="E6" s="102">
         <v>1</v>
       </c>
-      <c r="F6" s="103"/>
-      <c r="G6" s="103"/>
-      <c r="H6" s="103"/>
-      <c r="I6" s="103"/>
-      <c r="J6" s="103"/>
-      <c r="K6" s="103"/>
-      <c r="L6" s="103"/>
-      <c r="M6" s="103">
+      <c r="F6" s="102"/>
+      <c r="G6" s="102"/>
+      <c r="H6" s="102"/>
+      <c r="I6" s="102"/>
+      <c r="J6" s="102"/>
+      <c r="K6" s="102"/>
+      <c r="L6" s="102"/>
+      <c r="M6" s="102">
         <v>3</v>
       </c>
-      <c r="N6" s="103"/>
-      <c r="O6" s="103"/>
-      <c r="P6" s="103"/>
-      <c r="Q6" s="103"/>
-      <c r="R6" s="103"/>
-      <c r="S6" s="103"/>
-      <c r="T6" s="104">
+      <c r="N6" s="102"/>
+      <c r="O6" s="102"/>
+      <c r="P6" s="102"/>
+      <c r="Q6" s="102"/>
+      <c r="R6" s="102"/>
+      <c r="S6" s="102"/>
+      <c r="T6" s="103">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:20">
-      <c r="A7" s="96">
+    <row r="7" spans="1:22">
+      <c r="A7" s="95">
         <v>15</v>
       </c>
-      <c r="B7" s="102">
+      <c r="B7" s="101">
         <v>43904.625</v>
       </c>
-      <c r="C7" s="101" t="s">
+      <c r="C7" s="100" t="s">
         <v>19</v>
       </c>
-      <c r="D7" s="105">
+      <c r="D7" s="104">
         <v>2</v>
       </c>
-      <c r="E7" s="105">
+      <c r="E7" s="104">
         <v>1</v>
       </c>
-      <c r="F7" s="105"/>
-      <c r="G7" s="105"/>
-      <c r="H7" s="105"/>
-      <c r="I7" s="105"/>
-      <c r="J7" s="105"/>
-      <c r="K7" s="105"/>
-      <c r="L7" s="105"/>
-      <c r="M7" s="105">
+      <c r="F7" s="104"/>
+      <c r="G7" s="104"/>
+      <c r="H7" s="104"/>
+      <c r="I7" s="104"/>
+      <c r="J7" s="104"/>
+      <c r="K7" s="104"/>
+      <c r="L7" s="104"/>
+      <c r="M7" s="104">
         <v>5</v>
       </c>
-      <c r="N7" s="105"/>
-      <c r="O7" s="105"/>
-      <c r="P7" s="105"/>
-      <c r="Q7" s="105"/>
-      <c r="R7" s="105"/>
-      <c r="S7" s="105"/>
-      <c r="T7" s="106">
+      <c r="N7" s="104"/>
+      <c r="O7" s="104"/>
+      <c r="P7" s="104"/>
+      <c r="Q7" s="104"/>
+      <c r="R7" s="104"/>
+      <c r="S7" s="104"/>
+      <c r="T7" s="105">
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:20">
-      <c r="A8" s="107">
+    <row r="8" spans="1:22">
+      <c r="A8" s="106">
         <v>16</v>
       </c>
-      <c r="B8" s="102">
+      <c r="B8" s="101">
         <v>43905.625</v>
       </c>
-      <c r="C8" s="101" t="s">
+      <c r="C8" s="100" t="s">
         <v>19</v>
       </c>
-      <c r="D8" s="103">
+      <c r="D8" s="102">
         <v>3</v>
       </c>
-      <c r="E8" s="103">
+      <c r="E8" s="102">
         <v>4</v>
       </c>
-      <c r="F8" s="103"/>
-      <c r="G8" s="103"/>
-      <c r="H8" s="103"/>
-      <c r="I8" s="103"/>
-      <c r="J8" s="103"/>
-      <c r="K8" s="103"/>
-      <c r="L8" s="103"/>
-      <c r="M8" s="103">
+      <c r="F8" s="102"/>
+      <c r="G8" s="102"/>
+      <c r="H8" s="102"/>
+      <c r="I8" s="102"/>
+      <c r="J8" s="102"/>
+      <c r="K8" s="102"/>
+      <c r="L8" s="102"/>
+      <c r="M8" s="102">
         <v>5</v>
       </c>
-      <c r="N8" s="103"/>
-      <c r="O8" s="103"/>
-      <c r="P8" s="103"/>
-      <c r="Q8" s="103"/>
-      <c r="R8" s="103"/>
-      <c r="S8" s="103"/>
-      <c r="T8" s="104">
+      <c r="N8" s="102"/>
+      <c r="O8" s="102"/>
+      <c r="P8" s="102"/>
+      <c r="Q8" s="102"/>
+      <c r="R8" s="102"/>
+      <c r="S8" s="102"/>
+      <c r="T8" s="103">
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:20">
-      <c r="A9" s="108">
+    <row r="9" spans="1:22">
+      <c r="A9" s="107">
         <v>17</v>
       </c>
-      <c r="B9" s="102">
+      <c r="B9" s="101">
         <v>43906.625</v>
       </c>
-      <c r="C9" s="109" t="s">
+      <c r="C9" s="108" t="s">
         <v>19</v>
       </c>
-      <c r="D9" s="105">
+      <c r="D9" s="104">
         <v>3</v>
       </c>
-      <c r="E9" s="105">
+      <c r="E9" s="104">
         <v>5</v>
       </c>
-      <c r="F9" s="105"/>
-      <c r="G9" s="105"/>
-      <c r="H9" s="105"/>
-      <c r="I9" s="105"/>
-      <c r="J9" s="105"/>
-      <c r="K9" s="105"/>
-      <c r="L9" s="105"/>
-      <c r="M9" s="105">
+      <c r="F9" s="104"/>
+      <c r="G9" s="104"/>
+      <c r="H9" s="104"/>
+      <c r="I9" s="104"/>
+      <c r="J9" s="104"/>
+      <c r="K9" s="104"/>
+      <c r="L9" s="104"/>
+      <c r="M9" s="104">
         <v>5</v>
       </c>
-      <c r="N9" s="105"/>
-      <c r="O9" s="105"/>
-      <c r="P9" s="105"/>
-      <c r="Q9" s="105"/>
-      <c r="R9" s="105"/>
-      <c r="S9" s="105"/>
-      <c r="T9" s="106">
+      <c r="N9" s="104"/>
+      <c r="O9" s="104"/>
+      <c r="P9" s="104"/>
+      <c r="Q9" s="104"/>
+      <c r="R9" s="104"/>
+      <c r="S9" s="104"/>
+      <c r="T9" s="105">
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:20">
-      <c r="A10" s="108">
+    <row r="10" spans="1:22">
+      <c r="A10" s="107">
         <v>18</v>
       </c>
-      <c r="B10" s="102">
+      <c r="B10" s="101">
         <v>43907.625</v>
       </c>
-      <c r="C10" s="109" t="s">
+      <c r="C10" s="108" t="s">
         <v>41</v>
       </c>
-      <c r="D10" s="105">
+      <c r="D10" s="104">
         <v>2</v>
       </c>
-      <c r="E10" s="105">
+      <c r="E10" s="104">
         <v>4</v>
       </c>
-      <c r="F10" s="105">
+      <c r="F10" s="104">
         <v>0</v>
       </c>
-      <c r="G10" s="105">
+      <c r="G10" s="104">
         <v>0</v>
       </c>
-      <c r="H10" s="105">
+      <c r="H10" s="104">
         <v>0</v>
       </c>
-      <c r="I10" s="105">
+      <c r="I10" s="104">
         <v>0</v>
       </c>
-      <c r="J10" s="105">
+      <c r="J10" s="104">
         <v>0</v>
       </c>
-      <c r="K10" s="105">
+      <c r="K10" s="104">
         <v>0</v>
       </c>
-      <c r="L10" s="105">
+      <c r="L10" s="104">
         <v>0</v>
       </c>
-      <c r="M10" s="105">
+      <c r="M10" s="104">
         <v>6</v>
       </c>
-      <c r="N10" s="105">
+      <c r="N10" s="104">
         <v>0</v>
       </c>
-      <c r="O10" s="105">
+      <c r="O10" s="104">
         <v>0</v>
       </c>
-      <c r="P10" s="105">
+      <c r="P10" s="104">
         <v>0</v>
       </c>
-      <c r="Q10" s="105">
+      <c r="Q10" s="104">
         <v>0</v>
       </c>
-      <c r="R10" s="105">
+      <c r="R10" s="104">
         <v>0</v>
       </c>
-      <c r="S10" s="105">
+      <c r="S10" s="104">
         <v>0</v>
       </c>
-      <c r="T10" s="106">
+      <c r="T10" s="105">
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:20">
-      <c r="A11" s="108">
+    <row r="11" spans="1:22">
+      <c r="A11" s="107">
         <v>19</v>
       </c>
-      <c r="B11" s="110">
+      <c r="B11" s="109">
         <v>43908</v>
       </c>
-      <c r="C11" s="109" t="s">
+      <c r="C11" s="108" t="s">
         <v>41</v>
       </c>
-      <c r="D11" s="105">
+      <c r="D11" s="104">
         <v>2</v>
       </c>
-      <c r="E11" s="105">
+      <c r="E11" s="104">
         <v>4</v>
       </c>
-      <c r="F11" s="105">
+      <c r="F11" s="104">
         <v>0</v>
       </c>
-      <c r="G11" s="105">
+      <c r="G11" s="104">
         <v>0</v>
       </c>
-      <c r="H11" s="105">
+      <c r="H11" s="104">
         <v>0</v>
       </c>
-      <c r="I11" s="105">
+      <c r="I11" s="104">
         <v>0</v>
       </c>
-      <c r="J11" s="105">
+      <c r="J11" s="104">
         <v>0</v>
       </c>
-      <c r="K11" s="105">
+      <c r="K11" s="104">
         <v>0</v>
       </c>
-      <c r="L11" s="105">
+      <c r="L11" s="104">
         <v>0</v>
       </c>
-      <c r="M11" s="105">
+      <c r="M11" s="104">
         <v>6</v>
       </c>
-      <c r="N11" s="105">
+      <c r="N11" s="104">
         <v>0</v>
       </c>
-      <c r="O11" s="105">
+      <c r="O11" s="104">
         <v>0</v>
       </c>
-      <c r="P11" s="105">
+      <c r="P11" s="104">
         <v>0</v>
       </c>
-      <c r="Q11" s="105">
+      <c r="Q11" s="104">
         <v>0</v>
       </c>
-      <c r="R11" s="105">
+      <c r="R11" s="104">
         <v>0</v>
       </c>
-      <c r="S11" s="105">
+      <c r="S11" s="104">
         <v>0</v>
       </c>
-      <c r="T11" s="106">
+      <c r="T11" s="105">
         <v>12</v>
       </c>
     </row>
-    <row r="12" spans="1:20">
-      <c r="A12" s="108">
+    <row r="12" spans="1:22">
+      <c r="A12" s="107">
         <v>20</v>
       </c>
-      <c r="B12" s="110">
+      <c r="B12" s="109">
         <v>43909</v>
       </c>
-      <c r="C12" s="109" t="s">
+      <c r="C12" s="108" t="s">
         <v>41</v>
       </c>
-      <c r="D12" s="105">
+      <c r="D12" s="104">
         <v>6</v>
       </c>
-      <c r="E12" s="105">
+      <c r="E12" s="104">
         <v>8</v>
       </c>
-      <c r="F12" s="105">
+      <c r="F12" s="104">
         <v>0</v>
       </c>
-      <c r="G12" s="105">
+      <c r="G12" s="104">
         <v>0</v>
       </c>
-      <c r="H12" s="105">
+      <c r="H12" s="104">
         <v>0</v>
       </c>
-      <c r="I12" s="105">
+      <c r="I12" s="104">
         <v>0</v>
       </c>
-      <c r="J12" s="105">
+      <c r="J12" s="104">
         <v>0</v>
       </c>
-      <c r="K12" s="105">
+      <c r="K12" s="104">
         <v>0</v>
       </c>
-      <c r="L12" s="105">
+      <c r="L12" s="104">
         <v>0</v>
       </c>
-      <c r="M12" s="105">
+      <c r="M12" s="104">
         <v>6</v>
       </c>
-      <c r="N12" s="105">
+      <c r="N12" s="104">
         <v>0</v>
       </c>
-      <c r="O12" s="105">
+      <c r="O12" s="104">
         <v>0</v>
       </c>
-      <c r="P12" s="105">
+      <c r="P12" s="104">
         <v>0</v>
       </c>
-      <c r="Q12" s="105">
+      <c r="Q12" s="104">
         <v>0</v>
       </c>
-      <c r="R12" s="105">
+      <c r="R12" s="104">
         <v>0</v>
       </c>
-      <c r="S12" s="105">
+      <c r="S12" s="104">
         <v>0</v>
       </c>
-      <c r="T12" s="106">
+      <c r="T12" s="105">
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="1:20">
-      <c r="A13" s="108">
+    <row r="13" spans="1:22">
+      <c r="A13" s="107">
         <v>21</v>
       </c>
-      <c r="B13" s="110">
+      <c r="B13" s="109">
         <v>43910</v>
       </c>
-      <c r="C13" s="109" t="s">
+      <c r="C13" s="108" t="s">
         <v>41</v>
       </c>
-      <c r="D13" s="105">
+      <c r="D13" s="104">
         <v>10</v>
       </c>
-      <c r="E13" s="105">
+      <c r="E13" s="104">
         <v>12</v>
       </c>
-      <c r="F13" s="105">
+      <c r="F13" s="104">
         <v>0</v>
       </c>
-      <c r="G13" s="105">
+      <c r="G13" s="104">
         <v>0</v>
       </c>
-      <c r="H13" s="105">
+      <c r="H13" s="104">
         <v>0</v>
       </c>
-      <c r="I13" s="105">
+      <c r="I13" s="104">
         <v>0</v>
       </c>
-      <c r="J13" s="105">
+      <c r="J13" s="104">
         <v>1</v>
       </c>
-      <c r="K13" s="105">
+      <c r="K13" s="104">
         <v>0</v>
       </c>
-      <c r="L13" s="105">
+      <c r="L13" s="104">
         <v>0</v>
       </c>
-      <c r="M13" s="105">
+      <c r="M13" s="104">
         <v>6</v>
       </c>
-      <c r="N13" s="105">
+      <c r="N13" s="104">
         <v>1</v>
       </c>
-      <c r="O13" s="105">
+      <c r="O13" s="104">
         <v>0</v>
       </c>
-      <c r="P13" s="105">
+      <c r="P13" s="104">
         <v>0</v>
       </c>
-      <c r="Q13" s="105">
+      <c r="Q13" s="104">
         <v>0</v>
       </c>
-      <c r="R13" s="105">
+      <c r="R13" s="104">
         <v>1</v>
       </c>
-      <c r="S13" s="105">
+      <c r="S13" s="104">
         <v>0</v>
       </c>
-      <c r="T13" s="106">
+      <c r="T13" s="105">
         <v>31</v>
       </c>
+    </row>
+    <row r="14" spans="1:22">
+      <c r="A14" s="107">
+        <v>22</v>
+      </c>
+      <c r="B14" s="109">
+        <v>43911</v>
+      </c>
+      <c r="C14" s="108" t="s">
+        <v>41</v>
+      </c>
+      <c r="D14" s="113">
+        <v>16</v>
+      </c>
+      <c r="E14" s="113">
+        <v>19</v>
+      </c>
+      <c r="F14" s="113">
+        <v>1</v>
+      </c>
+      <c r="G14" s="113">
+        <v>0</v>
+      </c>
+      <c r="H14" s="113">
+        <v>0</v>
+      </c>
+      <c r="I14" s="113">
+        <v>0</v>
+      </c>
+      <c r="J14" s="113">
+        <v>2</v>
+      </c>
+      <c r="K14" s="113">
+        <v>0</v>
+      </c>
+      <c r="L14" s="113">
+        <v>0</v>
+      </c>
+      <c r="M14" s="113">
+        <v>6</v>
+      </c>
+      <c r="N14" s="113">
+        <v>1</v>
+      </c>
+      <c r="O14" s="113">
+        <v>0</v>
+      </c>
+      <c r="P14" s="113">
+        <v>0</v>
+      </c>
+      <c r="Q14" s="113">
+        <v>0</v>
+      </c>
+      <c r="R14" s="113">
+        <v>1</v>
+      </c>
+      <c r="S14" s="113">
+        <v>0</v>
+      </c>
+      <c r="T14" s="113">
+        <v>46</v>
+      </c>
+      <c r="U14" s="114"/>
+      <c r="V14" s="115"/>
     </row>
     <row r="20" spans="2:19">
       <c r="B20" s="18"/>

</xml_diff>